<commit_message>
implemented ASL, LSR, ROL, and ROR instructions
</commit_message>
<xml_diff>
--- a/docs/PandesalCPU Specs.xlsx
+++ b/docs/PandesalCPU Specs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shim Manaloto\Documents\PandesalCPU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shim Manaloto\Documents\PandesalCPU\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C8574D2-B5D8-4334-9717-0FC84702EBE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CF45D77-54B7-4B97-8422-32A8413BE51F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{A2A5A835-37AC-4F29-881C-332D1F6F724B}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1123" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1240" uniqueCount="390">
   <si>
     <t>Microcode</t>
   </si>
@@ -1139,6 +1139,75 @@
   </si>
   <si>
     <t>0000 0000 001 1 1 0 1 0</t>
+  </si>
+  <si>
+    <t>Memory Layout</t>
+  </si>
+  <si>
+    <t>RAM</t>
+  </si>
+  <si>
+    <t>0x0000 - 0x7FFF</t>
+  </si>
+  <si>
+    <t>Memory-mapped Display</t>
+  </si>
+  <si>
+    <t>0x8000 - 0xBFFF</t>
+  </si>
+  <si>
+    <t>ASL A</t>
+  </si>
+  <si>
+    <t>LSR A</t>
+  </si>
+  <si>
+    <t>ROL A</t>
+  </si>
+  <si>
+    <t>ROR A</t>
+  </si>
+  <si>
+    <t>ASL abs</t>
+  </si>
+  <si>
+    <t>LSR abs</t>
+  </si>
+  <si>
+    <t>ROL abs</t>
+  </si>
+  <si>
+    <t>ROR abs</t>
+  </si>
+  <si>
+    <t>0101 0110 110 1 1 0 1 0</t>
+  </si>
+  <si>
+    <t>0101 0110 111 1 1 0 1 0</t>
+  </si>
+  <si>
+    <t>0101 0110 110 1 0 0 1 0</t>
+  </si>
+  <si>
+    <t>0101 0110 111 1 0 0 1 0</t>
+  </si>
+  <si>
+    <t>0101 0110 110 1 1 0 0 0</t>
+  </si>
+  <si>
+    <t>0101 0110 111 1 1 0 0 0</t>
+  </si>
+  <si>
+    <t>0101 0110 110 1 0 0 0 0</t>
+  </si>
+  <si>
+    <t>0101 0110 111 1 0 0 0 0</t>
+  </si>
+  <si>
+    <t>1111 0110 000 0 0 0 0 0</t>
+  </si>
+  <si>
+    <t>0111 0111 000 0 0 0 1 1</t>
   </si>
 </sst>
 </file>
@@ -1704,10 +1773,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E48F8AD-971A-4094-8D85-72B0AE25E8BF}">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView zoomScale="98" workbookViewId="0">
-      <selection activeCell="N43" sqref="N43"/>
+    <sheetView zoomScale="96" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1720,7 +1789,9 @@
     <col min="6" max="6" width="5.81640625" customWidth="1"/>
     <col min="7" max="7" width="3.453125" customWidth="1"/>
     <col min="8" max="8" width="6.54296875" customWidth="1"/>
-    <col min="11" max="11" width="27.7265625" customWidth="1"/>
+    <col min="9" max="9" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.36328125" bestFit="1" customWidth="1"/>
     <col min="20" max="21" width="10.26953125" customWidth="1"/>
     <col min="22" max="22" width="10.7265625" customWidth="1"/>
     <col min="23" max="23" width="10.36328125" customWidth="1"/>
@@ -1737,12 +1808,15 @@
     <col min="35" max="35" width="10.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="J1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1767,8 +1841,14 @@
       <c r="H2" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="J2" t="s">
+        <v>368</v>
+      </c>
+      <c r="K2" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1793,19 +1873,25 @@
       <c r="H3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="J3" t="s">
+        <v>369</v>
+      </c>
+      <c r="K3" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="18.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" ht="18.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>95</v>
       </c>
@@ -1813,7 +1899,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>96</v>
       </c>
@@ -1830,7 +1916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>97</v>
       </c>
@@ -1847,7 +1933,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>98</v>
       </c>
@@ -1864,7 +1950,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>105</v>
       </c>
@@ -1881,7 +1967,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>100</v>
       </c>
@@ -1898,7 +1984,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -1915,7 +2001,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>99</v>
       </c>
@@ -1932,7 +2018,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>101</v>
       </c>
@@ -2106,8 +2192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC51F965-835D-4E82-9AC8-2752CA30592B}">
   <dimension ref="A1:AJ86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D31" zoomScale="98" zoomScaleNormal="101" workbookViewId="0">
-      <selection activeCell="G51" sqref="G51"/>
+    <sheetView tabSelected="1" topLeftCell="E29" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
+      <selection activeCell="J52" sqref="J52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4703,7 +4789,9 @@
       <c r="A46" s="16" t="s">
         <v>326</v>
       </c>
-      <c r="B46" s="11"/>
+      <c r="B46" s="11" t="s">
+        <v>372</v>
+      </c>
       <c r="C46" s="11" t="s">
         <v>112</v>
       </c>
@@ -4713,25 +4801,53 @@
       <c r="E46" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="F46" s="11"/>
-      <c r="G46" s="11"/>
-      <c r="H46" s="11"/>
-      <c r="I46" s="11"/>
-      <c r="J46" s="11"/>
-      <c r="K46" s="11"/>
-      <c r="L46" s="11"/>
-      <c r="M46" s="11"/>
-      <c r="N46" s="11"/>
-      <c r="O46" s="11"/>
-      <c r="P46" s="11"/>
-      <c r="Q46" s="11"/>
-      <c r="R46" s="10"/>
+      <c r="F46" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="G46" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="H46" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="I46" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="J46" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="K46" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="L46" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="M46" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="N46" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="O46" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="P46" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q46" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="R46" s="12" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A47" s="16" t="s">
         <v>327</v>
       </c>
-      <c r="B47" s="11"/>
+      <c r="B47" s="11" t="s">
+        <v>373</v>
+      </c>
       <c r="C47" s="11" t="s">
         <v>112</v>
       </c>
@@ -4741,25 +4857,53 @@
       <c r="E47" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="F47" s="11"/>
-      <c r="G47" s="11"/>
-      <c r="H47" s="11"/>
-      <c r="I47" s="11"/>
-      <c r="J47" s="11"/>
-      <c r="K47" s="11"/>
-      <c r="L47" s="11"/>
-      <c r="M47" s="11"/>
-      <c r="N47" s="11"/>
-      <c r="O47" s="11"/>
-      <c r="P47" s="11"/>
-      <c r="Q47" s="11"/>
-      <c r="R47" s="10"/>
+      <c r="F47" s="11" t="s">
+        <v>381</v>
+      </c>
+      <c r="G47" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="H47" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="I47" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="J47" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="K47" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="L47" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="M47" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="N47" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="O47" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="P47" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q47" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="R47" s="12" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A48" s="16" t="s">
         <v>328</v>
       </c>
-      <c r="B48" s="11"/>
+      <c r="B48" s="11" t="s">
+        <v>374</v>
+      </c>
       <c r="C48" s="11" t="s">
         <v>112</v>
       </c>
@@ -4769,25 +4913,53 @@
       <c r="E48" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="F48" s="11"/>
-      <c r="G48" s="11"/>
-      <c r="H48" s="11"/>
-      <c r="I48" s="11"/>
-      <c r="J48" s="11"/>
-      <c r="K48" s="11"/>
-      <c r="L48" s="11"/>
-      <c r="M48" s="11"/>
-      <c r="N48" s="11"/>
-      <c r="O48" s="11"/>
-      <c r="P48" s="11"/>
-      <c r="Q48" s="11"/>
-      <c r="R48" s="10"/>
+      <c r="F48" s="11" t="s">
+        <v>382</v>
+      </c>
+      <c r="G48" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="H48" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="I48" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="J48" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="K48" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="L48" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="M48" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="N48" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="O48" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="P48" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q48" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="R48" s="12" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A49" s="16" t="s">
         <v>329</v>
       </c>
-      <c r="B49" s="11"/>
+      <c r="B49" s="11" t="s">
+        <v>375</v>
+      </c>
       <c r="C49" s="11" t="s">
         <v>112</v>
       </c>
@@ -4797,25 +4969,53 @@
       <c r="E49" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="F49" s="11"/>
-      <c r="G49" s="11"/>
-      <c r="H49" s="11"/>
-      <c r="I49" s="11"/>
-      <c r="J49" s="11"/>
-      <c r="K49" s="11"/>
-      <c r="L49" s="11"/>
-      <c r="M49" s="11"/>
-      <c r="N49" s="11"/>
-      <c r="O49" s="11"/>
-      <c r="P49" s="11"/>
-      <c r="Q49" s="11"/>
-      <c r="R49" s="10"/>
+      <c r="F49" s="11" t="s">
+        <v>383</v>
+      </c>
+      <c r="G49" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="H49" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="I49" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="J49" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="K49" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="L49" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="M49" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="N49" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="O49" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="P49" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q49" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="R49" s="12" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A50" s="16" t="s">
         <v>330</v>
       </c>
-      <c r="B50" s="11"/>
+      <c r="B50" s="11" t="s">
+        <v>376</v>
+      </c>
       <c r="C50" s="11" t="s">
         <v>112</v>
       </c>
@@ -4825,25 +5025,53 @@
       <c r="E50" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="F50" s="11"/>
-      <c r="G50" s="11"/>
-      <c r="H50" s="11"/>
-      <c r="I50" s="11"/>
-      <c r="J50" s="11"/>
-      <c r="K50" s="11"/>
-      <c r="L50" s="11"/>
-      <c r="M50" s="11"/>
-      <c r="N50" s="11"/>
-      <c r="O50" s="11"/>
-      <c r="P50" s="11"/>
-      <c r="Q50" s="11"/>
-      <c r="R50" s="10"/>
+      <c r="F50" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="G50" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="H50" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="I50" s="11" t="s">
+        <v>388</v>
+      </c>
+      <c r="J50" s="11" t="s">
+        <v>384</v>
+      </c>
+      <c r="K50" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="L50" s="11" t="s">
+        <v>389</v>
+      </c>
+      <c r="M50" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="N50" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="O50" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="P50" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q50" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="R50" s="12" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A51" s="16" t="s">
         <v>331</v>
       </c>
-      <c r="B51" s="11"/>
+      <c r="B51" s="11" t="s">
+        <v>377</v>
+      </c>
       <c r="C51" s="11" t="s">
         <v>112</v>
       </c>
@@ -4853,25 +5081,53 @@
       <c r="E51" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="F51" s="11"/>
-      <c r="G51" s="11"/>
-      <c r="H51" s="11"/>
-      <c r="I51" s="11"/>
-      <c r="J51" s="11"/>
-      <c r="K51" s="11"/>
-      <c r="L51" s="11"/>
-      <c r="M51" s="11"/>
-      <c r="N51" s="11"/>
-      <c r="O51" s="11"/>
-      <c r="P51" s="11"/>
-      <c r="Q51" s="11"/>
-      <c r="R51" s="10"/>
+      <c r="F51" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="G51" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="H51" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="I51" s="11" t="s">
+        <v>388</v>
+      </c>
+      <c r="J51" s="11" t="s">
+        <v>385</v>
+      </c>
+      <c r="K51" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="L51" s="11" t="s">
+        <v>389</v>
+      </c>
+      <c r="M51" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="N51" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="O51" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="P51" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q51" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="R51" s="12" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A52" s="16" t="s">
         <v>332</v>
       </c>
-      <c r="B52" s="11"/>
+      <c r="B52" s="11" t="s">
+        <v>378</v>
+      </c>
       <c r="C52" s="11" t="s">
         <v>112</v>
       </c>
@@ -4881,25 +5137,53 @@
       <c r="E52" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="F52" s="11"/>
-      <c r="G52" s="11"/>
-      <c r="H52" s="11"/>
-      <c r="I52" s="11"/>
-      <c r="J52" s="11"/>
-      <c r="K52" s="11"/>
-      <c r="L52" s="11"/>
-      <c r="M52" s="11"/>
-      <c r="N52" s="11"/>
-      <c r="O52" s="11"/>
-      <c r="P52" s="11"/>
-      <c r="Q52" s="11"/>
-      <c r="R52" s="10"/>
+      <c r="F52" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="G52" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="H52" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="I52" s="11" t="s">
+        <v>388</v>
+      </c>
+      <c r="J52" s="11" t="s">
+        <v>386</v>
+      </c>
+      <c r="K52" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="L52" s="11" t="s">
+        <v>389</v>
+      </c>
+      <c r="M52" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="N52" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="O52" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="P52" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q52" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="R52" s="12" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A53" s="16" t="s">
         <v>333</v>
       </c>
-      <c r="B53" s="11"/>
+      <c r="B53" s="11" t="s">
+        <v>379</v>
+      </c>
       <c r="C53" s="11" t="s">
         <v>112</v>
       </c>
@@ -4909,19 +5193,45 @@
       <c r="E53" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="F53" s="11"/>
-      <c r="G53" s="11"/>
-      <c r="H53" s="11"/>
-      <c r="I53" s="11"/>
-      <c r="J53" s="11"/>
-      <c r="K53" s="11"/>
-      <c r="L53" s="11"/>
-      <c r="M53" s="11"/>
-      <c r="N53" s="11"/>
-      <c r="O53" s="11"/>
-      <c r="P53" s="11"/>
-      <c r="Q53" s="11"/>
-      <c r="R53" s="10"/>
+      <c r="F53" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="G53" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="H53" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="I53" s="11" t="s">
+        <v>388</v>
+      </c>
+      <c r="J53" s="11" t="s">
+        <v>387</v>
+      </c>
+      <c r="K53" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="L53" s="11" t="s">
+        <v>389</v>
+      </c>
+      <c r="M53" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="N53" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="O53" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="P53" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q53" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="R53" s="12" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A54" s="16" t="s">

</xml_diff>

<commit_message>
implemented CPX and CPY instructions
</commit_message>
<xml_diff>
--- a/docs/PandesalCPU Specs.xlsx
+++ b/docs/PandesalCPU Specs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shim Manaloto\Documents\PandesalCPU\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CF45D77-54B7-4B97-8422-32A8413BE51F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{599B4860-11E9-4EED-92D0-69FF9ABED8E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{A2A5A835-37AC-4F29-881C-332D1F6F724B}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1240" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1296" uniqueCount="395">
   <si>
     <t>Microcode</t>
   </si>
@@ -1208,6 +1208,21 @@
   </si>
   <si>
     <t>0111 0111 000 0 0 0 1 1</t>
+  </si>
+  <si>
+    <t>CPY #</t>
+  </si>
+  <si>
+    <t>CPX #</t>
+  </si>
+  <si>
+    <t>CPY abs</t>
+  </si>
+  <si>
+    <t>CPX abs</t>
+  </si>
+  <si>
+    <t>0000 0000 001 1 1 0 1 1</t>
   </si>
 </sst>
 </file>
@@ -1776,7 +1791,7 @@
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView zoomScale="96" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2192,8 +2207,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC51F965-835D-4E82-9AC8-2752CA30592B}">
   <dimension ref="A1:AJ86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E29" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
-      <selection activeCell="J52" sqref="J52"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
+      <selection activeCell="F58" sqref="F58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5237,7 +5252,9 @@
       <c r="A54" s="16" t="s">
         <v>334</v>
       </c>
-      <c r="B54" s="11"/>
+      <c r="B54" s="11" t="s">
+        <v>391</v>
+      </c>
       <c r="C54" s="11" t="s">
         <v>112</v>
       </c>
@@ -5247,25 +5264,53 @@
       <c r="E54" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="F54" s="11"/>
-      <c r="G54" s="11"/>
-      <c r="H54" s="11"/>
-      <c r="I54" s="11"/>
-      <c r="J54" s="11"/>
-      <c r="K54" s="11"/>
-      <c r="L54" s="11"/>
-      <c r="M54" s="11"/>
-      <c r="N54" s="11"/>
-      <c r="O54" s="11"/>
-      <c r="P54" s="11"/>
-      <c r="Q54" s="11"/>
-      <c r="R54" s="10"/>
+      <c r="F54" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="G54" s="13" t="s">
+        <v>316</v>
+      </c>
+      <c r="H54" s="11" t="s">
+        <v>394</v>
+      </c>
+      <c r="I54" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="J54" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="K54" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="L54" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="M54" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="N54" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="O54" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="P54" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q54" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="R54" s="12" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A55" s="16" t="s">
         <v>335</v>
       </c>
-      <c r="B55" s="11"/>
+      <c r="B55" s="11" t="s">
+        <v>390</v>
+      </c>
       <c r="C55" s="11" t="s">
         <v>112</v>
       </c>
@@ -5275,25 +5320,53 @@
       <c r="E55" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="F55" s="11"/>
-      <c r="G55" s="11"/>
-      <c r="H55" s="11"/>
-      <c r="I55" s="11"/>
-      <c r="J55" s="11"/>
-      <c r="K55" s="11"/>
-      <c r="L55" s="11"/>
-      <c r="M55" s="11"/>
-      <c r="N55" s="11"/>
-      <c r="O55" s="11"/>
-      <c r="P55" s="11"/>
-      <c r="Q55" s="11"/>
-      <c r="R55" s="10"/>
+      <c r="F55" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="G55" s="13" t="s">
+        <v>315</v>
+      </c>
+      <c r="H55" s="11" t="s">
+        <v>394</v>
+      </c>
+      <c r="I55" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="J55" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="K55" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="L55" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="M55" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="N55" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="O55" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="P55" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q55" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="R55" s="12" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A56" s="16" t="s">
         <v>336</v>
       </c>
-      <c r="B56" s="11"/>
+      <c r="B56" s="11" t="s">
+        <v>393</v>
+      </c>
       <c r="C56" s="11" t="s">
         <v>112</v>
       </c>
@@ -5303,25 +5376,53 @@
       <c r="E56" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="F56" s="11"/>
-      <c r="G56" s="11"/>
-      <c r="H56" s="11"/>
-      <c r="I56" s="11"/>
-      <c r="J56" s="11"/>
-      <c r="K56" s="11"/>
-      <c r="L56" s="11"/>
-      <c r="M56" s="11"/>
-      <c r="N56" s="11"/>
-      <c r="O56" s="11"/>
-      <c r="P56" s="11"/>
-      <c r="Q56" s="11"/>
-      <c r="R56" s="10"/>
+      <c r="F56" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="G56" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="H56" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="I56" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="J56" s="11" t="s">
+        <v>316</v>
+      </c>
+      <c r="K56" s="11" t="s">
+        <v>366</v>
+      </c>
+      <c r="L56" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="M56" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="N56" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="O56" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="P56" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q56" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="R56" s="12" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A57" s="16" t="s">
         <v>337</v>
       </c>
-      <c r="B57" s="11"/>
+      <c r="B57" s="11" t="s">
+        <v>392</v>
+      </c>
       <c r="C57" s="11" t="s">
         <v>112</v>
       </c>
@@ -5331,25 +5432,50 @@
       <c r="E57" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="F57" s="11"/>
-      <c r="G57" s="11"/>
-      <c r="H57" s="11"/>
-      <c r="I57" s="11"/>
-      <c r="J57" s="11"/>
-      <c r="K57" s="11"/>
-      <c r="L57" s="11"/>
-      <c r="M57" s="11"/>
-      <c r="N57" s="11"/>
-      <c r="O57" s="11"/>
-      <c r="P57" s="11"/>
-      <c r="Q57" s="11"/>
-      <c r="R57" s="10"/>
+      <c r="F57" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="G57" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="H57" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="I57" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="J57" s="11" t="s">
+        <v>315</v>
+      </c>
+      <c r="K57" s="11" t="s">
+        <v>366</v>
+      </c>
+      <c r="L57" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="M57" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="N57" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="O57" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="P57" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q57" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="R57" s="12" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A58" s="16" t="s">
         <v>338</v>
       </c>
-      <c r="B58" s="11"/>
       <c r="C58" s="11" t="s">
         <v>112</v>
       </c>

</xml_diff>

<commit_message>
implemented LDX abs and LDY abs instructions
</commit_message>
<xml_diff>
--- a/docs/PandesalCPU Specs.xlsx
+++ b/docs/PandesalCPU Specs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shim Manaloto\Documents\PandesalCPU\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{599B4860-11E9-4EED-92D0-69FF9ABED8E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABD760D5-F87E-4ACB-BB26-D1F9E219EC56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{A2A5A835-37AC-4F29-881C-332D1F6F724B}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1296" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1324" uniqueCount="397">
   <si>
     <t>Microcode</t>
   </si>
@@ -1223,6 +1223,12 @@
   </si>
   <si>
     <t>0000 0000 001 1 1 0 1 1</t>
+  </si>
+  <si>
+    <t>LDX abs</t>
+  </si>
+  <si>
+    <t>LDY abs</t>
   </si>
 </sst>
 </file>
@@ -1399,7 +1405,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1444,6 +1450,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2207,8 +2214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC51F965-835D-4E82-9AC8-2752CA30592B}">
   <dimension ref="A1:AJ86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
-      <selection activeCell="F58" sqref="F58"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
+      <selection activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5476,6 +5483,9 @@
       <c r="A58" s="16" t="s">
         <v>338</v>
       </c>
+      <c r="B58" s="22" t="s">
+        <v>395</v>
+      </c>
       <c r="C58" s="11" t="s">
         <v>112</v>
       </c>
@@ -5485,25 +5495,53 @@
       <c r="E58" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="F58" s="11"/>
-      <c r="G58" s="11"/>
-      <c r="H58" s="11"/>
-      <c r="I58" s="11"/>
-      <c r="J58" s="11"/>
-      <c r="K58" s="11"/>
-      <c r="L58" s="11"/>
-      <c r="M58" s="11"/>
-      <c r="N58" s="11"/>
-      <c r="O58" s="11"/>
-      <c r="P58" s="11"/>
-      <c r="Q58" s="11"/>
-      <c r="R58" s="10"/>
+      <c r="F58" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="G58" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="H58" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="I58" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="J58" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="K58" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="L58" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="M58" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="N58" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="O58" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="P58" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q58" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="R58" s="12" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A59" s="16" t="s">
         <v>339</v>
       </c>
-      <c r="B59" s="11"/>
+      <c r="B59" s="11" t="s">
+        <v>396</v>
+      </c>
       <c r="C59" s="11" t="s">
         <v>112</v>
       </c>
@@ -5513,19 +5551,45 @@
       <c r="E59" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="F59" s="11"/>
-      <c r="G59" s="11"/>
-      <c r="H59" s="11"/>
-      <c r="I59" s="11"/>
-      <c r="J59" s="11"/>
-      <c r="K59" s="11"/>
-      <c r="L59" s="11"/>
-      <c r="M59" s="11"/>
-      <c r="N59" s="11"/>
-      <c r="O59" s="11"/>
-      <c r="P59" s="11"/>
-      <c r="Q59" s="11"/>
-      <c r="R59" s="10"/>
+      <c r="F59" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="G59" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="H59" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="I59" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="J59" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="K59" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="L59" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="M59" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="N59" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="O59" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="P59" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q59" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="R59" s="12" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A60" s="16" t="s">

</xml_diff>

<commit_message>
implemented LDA abs,x and LDA abs,y instructions
</commit_message>
<xml_diff>
--- a/docs/PandesalCPU Specs.xlsx
+++ b/docs/PandesalCPU Specs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shim Manaloto\Documents\PandesalCPU\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABD760D5-F87E-4ACB-BB26-D1F9E219EC56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F52ED72-7BF9-486F-84F8-6C7E6BD75DB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{A2A5A835-37AC-4F29-881C-332D1F6F724B}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1324" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1356" uniqueCount="407">
   <si>
     <t>Microcode</t>
   </si>
@@ -1229,6 +1229,36 @@
   </si>
   <si>
     <t>LDY abs</t>
+  </si>
+  <si>
+    <t>LDA abs,X</t>
+  </si>
+  <si>
+    <t>AND abs,Y</t>
+  </si>
+  <si>
+    <t>STA abs,Y</t>
+  </si>
+  <si>
+    <t>LDA abs,Y</t>
+  </si>
+  <si>
+    <t>AND abs,X</t>
+  </si>
+  <si>
+    <t>STA abs,X</t>
+  </si>
+  <si>
+    <t>1001 0111 000 0 0 0 0 0</t>
+  </si>
+  <si>
+    <t>1111 0110 000 0 0 0 0 1</t>
+  </si>
+  <si>
+    <t>0101 0110 000 1 1 0 1 0</t>
+  </si>
+  <si>
+    <t>1010 0111 000 0 0 0 0 0</t>
   </si>
 </sst>
 </file>
@@ -2214,8 +2244,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC51F965-835D-4E82-9AC8-2752CA30592B}">
   <dimension ref="A1:AJ86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
-      <selection activeCell="F60" sqref="F60"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="86" zoomScaleNormal="81" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5595,7 +5625,9 @@
       <c r="A60" s="16" t="s">
         <v>342</v>
       </c>
-      <c r="B60" s="11"/>
+      <c r="B60" s="11" t="s">
+        <v>397</v>
+      </c>
       <c r="C60" s="11" t="s">
         <v>112</v>
       </c>
@@ -5605,25 +5637,53 @@
       <c r="E60" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="F60" s="11"/>
-      <c r="G60" s="11"/>
-      <c r="H60" s="11"/>
-      <c r="I60" s="11"/>
-      <c r="J60" s="11"/>
-      <c r="K60" s="11"/>
-      <c r="L60" s="11"/>
-      <c r="M60" s="11"/>
-      <c r="N60" s="11"/>
-      <c r="O60" s="11"/>
-      <c r="P60" s="11"/>
-      <c r="Q60" s="11"/>
-      <c r="R60" s="10"/>
+      <c r="F60" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="G60" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="H60" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="I60" s="11" t="s">
+        <v>404</v>
+      </c>
+      <c r="J60" s="11" t="s">
+        <v>403</v>
+      </c>
+      <c r="K60" s="11" t="s">
+        <v>405</v>
+      </c>
+      <c r="L60" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="M60" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="N60" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="O60" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="P60" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q60" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="R60" s="12" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A61" s="16" t="s">
         <v>343</v>
       </c>
-      <c r="B61" s="11"/>
+      <c r="B61" s="22" t="s">
+        <v>400</v>
+      </c>
       <c r="C61" s="11" t="s">
         <v>112</v>
       </c>
@@ -5633,25 +5693,53 @@
       <c r="E61" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="F61" s="11"/>
-      <c r="G61" s="11"/>
-      <c r="H61" s="11"/>
-      <c r="I61" s="11"/>
-      <c r="J61" s="11"/>
-      <c r="K61" s="11"/>
-      <c r="L61" s="11"/>
-      <c r="M61" s="11"/>
-      <c r="N61" s="11"/>
-      <c r="O61" s="11"/>
-      <c r="P61" s="11"/>
-      <c r="Q61" s="11"/>
-      <c r="R61" s="10"/>
+      <c r="F61" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="G61" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="H61" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="I61" s="11" t="s">
+        <v>404</v>
+      </c>
+      <c r="J61" s="11" t="s">
+        <v>406</v>
+      </c>
+      <c r="K61" s="11" t="s">
+        <v>405</v>
+      </c>
+      <c r="L61" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="M61" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="N61" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="O61" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="P61" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q61" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="R61" s="12" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A62" s="16" t="s">
         <v>344</v>
       </c>
-      <c r="B62" s="11"/>
+      <c r="B62" s="22" t="s">
+        <v>401</v>
+      </c>
       <c r="C62" s="11" t="s">
         <v>112</v>
       </c>
@@ -5679,7 +5767,9 @@
       <c r="A63" s="16" t="s">
         <v>345</v>
       </c>
-      <c r="B63" s="11"/>
+      <c r="B63" s="11" t="s">
+        <v>398</v>
+      </c>
       <c r="C63" s="11" t="s">
         <v>112</v>
       </c>
@@ -5707,7 +5797,9 @@
       <c r="A64" s="16" t="s">
         <v>346</v>
       </c>
-      <c r="B64" s="11"/>
+      <c r="B64" s="22" t="s">
+        <v>402</v>
+      </c>
       <c r="C64" s="11" t="s">
         <v>112</v>
       </c>
@@ -5735,7 +5827,9 @@
       <c r="A65" s="16" t="s">
         <v>347</v>
       </c>
-      <c r="B65" s="11"/>
+      <c r="B65" s="11" t="s">
+        <v>399</v>
+      </c>
       <c r="C65" s="11" t="s">
         <v>112</v>
       </c>

</xml_diff>

<commit_message>
fix: fixed LDA abs,x and LDA abs,y microcode implementation
</commit_message>
<xml_diff>
--- a/docs/PandesalCPU Specs.xlsx
+++ b/docs/PandesalCPU Specs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shim Manaloto\Documents\PandesalCPU\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F52ED72-7BF9-486F-84F8-6C7E6BD75DB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC10267-0F33-4864-84D3-FCFD65FB64F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{A2A5A835-37AC-4F29-881C-332D1F6F724B}"/>
   </bookViews>
@@ -1249,16 +1249,16 @@
     <t>STA abs,X</t>
   </si>
   <si>
-    <t>1001 0111 000 0 0 0 0 0</t>
-  </si>
-  <si>
-    <t>1111 0110 000 0 0 0 0 1</t>
-  </si>
-  <si>
-    <t>0101 0110 000 1 1 0 1 0</t>
-  </si>
-  <si>
-    <t>1010 0111 000 0 0 0 0 0</t>
+    <t>0101 0001 000 0 0 0 0 0</t>
+  </si>
+  <si>
+    <t>0000 0101 000 1 0 0 0 0</t>
+  </si>
+  <si>
+    <t>0101 0001 000 0 1 0 0 0</t>
+  </si>
+  <si>
+    <t>0000 0000 000 1 1 0 0 0</t>
   </si>
 </sst>
 </file>
@@ -2244,8 +2244,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC51F965-835D-4E82-9AC8-2752CA30592B}">
   <dimension ref="A1:AJ86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="86" zoomScaleNormal="81" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="80" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F62" sqref="F62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5513,7 +5513,7 @@
       <c r="A58" s="16" t="s">
         <v>338</v>
       </c>
-      <c r="B58" s="22" t="s">
+      <c r="B58" s="13" t="s">
         <v>395</v>
       </c>
       <c r="C58" s="11" t="s">
@@ -5638,28 +5638,28 @@
         <v>132</v>
       </c>
       <c r="F60" s="11" t="s">
+        <v>316</v>
+      </c>
+      <c r="G60" s="22" t="s">
         <v>138</v>
       </c>
-      <c r="G60" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="H60" s="11" t="s">
-        <v>198</v>
-      </c>
-      <c r="I60" s="11" t="s">
+      <c r="H60" s="22" t="s">
+        <v>406</v>
+      </c>
+      <c r="I60" s="22" t="s">
+        <v>388</v>
+      </c>
+      <c r="J60" s="22" t="s">
+        <v>403</v>
+      </c>
+      <c r="K60" s="11" t="s">
         <v>404</v>
       </c>
-      <c r="J60" s="11" t="s">
-        <v>403</v>
-      </c>
-      <c r="K60" s="11" t="s">
+      <c r="L60" s="11" t="s">
         <v>405</v>
       </c>
-      <c r="L60" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="M60" s="12" t="s">
-        <v>135</v>
+      <c r="M60" s="11" t="s">
+        <v>142</v>
       </c>
       <c r="N60" s="12" t="s">
         <v>135</v>
@@ -5681,7 +5681,7 @@
       <c r="A61" s="16" t="s">
         <v>343</v>
       </c>
-      <c r="B61" s="22" t="s">
+      <c r="B61" s="13" t="s">
         <v>400</v>
       </c>
       <c r="C61" s="11" t="s">
@@ -5694,28 +5694,28 @@
         <v>132</v>
       </c>
       <c r="F61" s="11" t="s">
+        <v>315</v>
+      </c>
+      <c r="G61" s="22" t="s">
         <v>138</v>
       </c>
-      <c r="G61" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="H61" s="11" t="s">
-        <v>198</v>
-      </c>
-      <c r="I61" s="11" t="s">
+      <c r="H61" s="22" t="s">
+        <v>406</v>
+      </c>
+      <c r="I61" s="22" t="s">
+        <v>388</v>
+      </c>
+      <c r="J61" s="22" t="s">
+        <v>403</v>
+      </c>
+      <c r="K61" s="11" t="s">
         <v>404</v>
       </c>
-      <c r="J61" s="11" t="s">
-        <v>406</v>
-      </c>
-      <c r="K61" s="11" t="s">
+      <c r="L61" s="11" t="s">
         <v>405</v>
       </c>
-      <c r="L61" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="M61" s="12" t="s">
-        <v>135</v>
+      <c r="M61" s="11" t="s">
+        <v>142</v>
       </c>
       <c r="N61" s="12" t="s">
         <v>135</v>
@@ -5737,7 +5737,7 @@
       <c r="A62" s="16" t="s">
         <v>344</v>
       </c>
-      <c r="B62" s="22" t="s">
+      <c r="B62" s="13" t="s">
         <v>401</v>
       </c>
       <c r="C62" s="11" t="s">
@@ -5797,7 +5797,7 @@
       <c r="A64" s="16" t="s">
         <v>346</v>
       </c>
-      <c r="B64" s="22" t="s">
+      <c r="B64" s="13" t="s">
         <v>402</v>
       </c>
       <c r="C64" s="11" t="s">

</xml_diff>

<commit_message>
feat: implement LDA abs,X and LDA abs,Y instructions
</commit_message>
<xml_diff>
--- a/docs/PandesalCPU Specs.xlsx
+++ b/docs/PandesalCPU Specs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shim Manaloto\Documents\PandesalCPU\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00BF5280-6559-4221-94BB-3818B19167DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A03FBBB-A4B6-45E2-A06E-78FDE9104B1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{A2A5A835-37AC-4F29-881C-332D1F6F724B}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1497" uniqueCount="546">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1505" uniqueCount="547">
   <si>
     <t>000</t>
   </si>
@@ -1676,6 +1676,9 @@
   </si>
   <si>
     <t>FF</t>
+  </si>
+  <si>
+    <t>1010 1010 000 0 0 11 0</t>
   </si>
 </sst>
 </file>
@@ -2245,7 +2248,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E48F8AD-971A-4094-8D85-72B0AE25E8BF}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView zoomScale="114" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="114" workbookViewId="0">
       <selection activeCell="G6" sqref="A1:G6"/>
     </sheetView>
   </sheetViews>
@@ -2667,8 +2670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC51F965-835D-4E82-9AC8-2752CA30592B}">
   <dimension ref="A1:AJ257"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="72" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="D48" zoomScale="98" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I62" sqref="I62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6112,7 +6115,7 @@
       <c r="A61" s="12" t="s">
         <v>238</v>
       </c>
-      <c r="B61" s="16" t="s">
+      <c r="B61" s="15" t="s">
         <v>283</v>
       </c>
       <c r="C61" s="9" t="s">
@@ -6124,14 +6127,30 @@
       <c r="E61" s="9" t="s">
         <v>290</v>
       </c>
-      <c r="F61" s="9"/>
-      <c r="G61" s="9"/>
-      <c r="H61" s="9"/>
-      <c r="I61" s="9"/>
-      <c r="J61" s="9"/>
-      <c r="K61" s="9"/>
-      <c r="L61" s="9"/>
-      <c r="M61" s="9"/>
+      <c r="F61" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="G61" s="9" t="s">
+        <v>321</v>
+      </c>
+      <c r="H61" s="9" t="s">
+        <v>337</v>
+      </c>
+      <c r="I61" s="9" t="s">
+        <v>546</v>
+      </c>
+      <c r="J61" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="K61" s="10" t="s">
+        <v>306</v>
+      </c>
+      <c r="L61" s="10" t="s">
+        <v>306</v>
+      </c>
+      <c r="M61" s="10" t="s">
+        <v>306</v>
+      </c>
       <c r="N61" s="10" t="s">
         <v>306</v>
       </c>
@@ -6152,7 +6171,7 @@
       <c r="A62" s="12" t="s">
         <v>239</v>
       </c>
-      <c r="B62" s="16" t="s">
+      <c r="B62" s="15" t="s">
         <v>284</v>
       </c>
       <c r="C62" s="9" t="s">

</xml_diff>

<commit_message>
feat: implement AND abs,X and AND abs,Y instructions
</commit_message>
<xml_diff>
--- a/docs/PandesalCPU Specs.xlsx
+++ b/docs/PandesalCPU Specs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shim Manaloto\Documents\PandesalCPU\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A03FBBB-A4B6-45E2-A06E-78FDE9104B1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44E3865A-12BC-48E5-8AAE-FD8D5D5D5B2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{A2A5A835-37AC-4F29-881C-332D1F6F724B}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1505" uniqueCount="547">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1531" uniqueCount="548">
   <si>
     <t>000</t>
   </si>
@@ -1679,6 +1679,9 @@
   </si>
   <si>
     <t>1010 1010 000 0 0 11 0</t>
+  </si>
+  <si>
+    <t>0101 0110 011 1 0 01 0</t>
   </si>
 </sst>
 </file>
@@ -2670,8 +2673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC51F965-835D-4E82-9AC8-2752CA30592B}">
   <dimension ref="A1:AJ257"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D48" zoomScale="98" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I62" sqref="I62"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="50" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H67" sqref="H67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6183,19 +6186,45 @@
       <c r="E62" s="9" t="s">
         <v>290</v>
       </c>
-      <c r="F62" s="9"/>
-      <c r="G62" s="9"/>
-      <c r="H62" s="9"/>
-      <c r="I62" s="9"/>
-      <c r="J62" s="9"/>
-      <c r="K62" s="9"/>
-      <c r="L62" s="9"/>
-      <c r="M62" s="9"/>
-      <c r="N62" s="9"/>
-      <c r="O62" s="9"/>
-      <c r="P62" s="9"/>
-      <c r="Q62" s="9"/>
-      <c r="R62" s="8"/>
+      <c r="F62" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="G62" s="9" t="s">
+        <v>321</v>
+      </c>
+      <c r="H62" s="9" t="s">
+        <v>337</v>
+      </c>
+      <c r="I62" s="9" t="s">
+        <v>369</v>
+      </c>
+      <c r="J62" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="K62" s="9" t="s">
+        <v>547</v>
+      </c>
+      <c r="L62" s="10" t="s">
+        <v>306</v>
+      </c>
+      <c r="M62" s="10" t="s">
+        <v>306</v>
+      </c>
+      <c r="N62" s="10" t="s">
+        <v>306</v>
+      </c>
+      <c r="O62" s="10" t="s">
+        <v>306</v>
+      </c>
+      <c r="P62" s="10" t="s">
+        <v>306</v>
+      </c>
+      <c r="Q62" s="10" t="s">
+        <v>306</v>
+      </c>
+      <c r="R62" s="10" t="s">
+        <v>306</v>
+      </c>
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A63" s="12" t="s">
@@ -6213,19 +6242,45 @@
       <c r="E63" s="9" t="s">
         <v>290</v>
       </c>
-      <c r="F63" s="9"/>
-      <c r="G63" s="9"/>
-      <c r="H63" s="9"/>
-      <c r="I63" s="9"/>
-      <c r="J63" s="9"/>
-      <c r="K63" s="9"/>
-      <c r="L63" s="9"/>
-      <c r="M63" s="9"/>
-      <c r="N63" s="9"/>
-      <c r="O63" s="9"/>
-      <c r="P63" s="9"/>
-      <c r="Q63" s="9"/>
-      <c r="R63" s="8"/>
+      <c r="F63" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="G63" s="9" t="s">
+        <v>321</v>
+      </c>
+      <c r="H63" s="9" t="s">
+        <v>337</v>
+      </c>
+      <c r="I63" s="9" t="s">
+        <v>546</v>
+      </c>
+      <c r="J63" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="K63" s="9" t="s">
+        <v>547</v>
+      </c>
+      <c r="L63" s="10" t="s">
+        <v>306</v>
+      </c>
+      <c r="M63" s="10" t="s">
+        <v>306</v>
+      </c>
+      <c r="N63" s="10" t="s">
+        <v>306</v>
+      </c>
+      <c r="O63" s="10" t="s">
+        <v>306</v>
+      </c>
+      <c r="P63" s="10" t="s">
+        <v>306</v>
+      </c>
+      <c r="Q63" s="10" t="s">
+        <v>306</v>
+      </c>
+      <c r="R63" s="10" t="s">
+        <v>306</v>
+      </c>
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A64" s="12" t="s">

</xml_diff>

<commit_message>
feat: implement INC A and INC abs instructions
</commit_message>
<xml_diff>
--- a/docs/PandesalCPU Specs.xlsx
+++ b/docs/PandesalCPU Specs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shim Manaloto\Documents\PandesalCPU\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D8B87C5-B1E2-428A-9C05-CD3DAAA014A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E963BAC0-11EC-45CF-B3B3-C3897E975D69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{A2A5A835-37AC-4F29-881C-332D1F6F724B}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1557" uniqueCount="550">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1585" uniqueCount="555">
   <si>
     <t>000</t>
   </si>
@@ -1688,6 +1688,21 @@
   </si>
   <si>
     <t>1010 1010 000 0 0 11 1</t>
+  </si>
+  <si>
+    <t>INC A</t>
+  </si>
+  <si>
+    <t>INC abs</t>
+  </si>
+  <si>
+    <t>0101 0110 000 1 1 01 0</t>
+  </si>
+  <si>
+    <t>0000 000 000 0 0 01 1</t>
+  </si>
+  <si>
+    <t>0101 1111 000 1 1 00 0</t>
   </si>
 </sst>
 </file>
@@ -2679,8 +2694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC51F965-835D-4E82-9AC8-2752CA30592B}">
   <dimension ref="A1:AJ257"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B67" sqref="B66:B67"/>
+    <sheetView tabSelected="1" topLeftCell="H54" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L67" sqref="L67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6404,7 +6419,9 @@
       <c r="A66" s="12" t="s">
         <v>234</v>
       </c>
-      <c r="B66" s="15"/>
+      <c r="B66" s="15" t="s">
+        <v>550</v>
+      </c>
       <c r="C66" s="9" t="s">
         <v>287</v>
       </c>
@@ -6414,25 +6431,53 @@
       <c r="E66" s="9" t="s">
         <v>289</v>
       </c>
-      <c r="F66" s="9"/>
-      <c r="G66" s="9"/>
-      <c r="H66" s="9"/>
-      <c r="I66" s="9"/>
-      <c r="J66" s="9"/>
-      <c r="K66" s="9"/>
-      <c r="L66" s="9"/>
-      <c r="M66" s="9"/>
-      <c r="N66" s="9"/>
-      <c r="O66" s="9"/>
-      <c r="P66" s="9"/>
-      <c r="Q66" s="9"/>
-      <c r="R66" s="9"/>
+      <c r="F66" s="9" t="s">
+        <v>329</v>
+      </c>
+      <c r="G66" s="9" t="s">
+        <v>552</v>
+      </c>
+      <c r="H66" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="I66" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="J66" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="K66" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="L66" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="M66" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="N66" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="O66" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="P66" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="Q66" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="R66" s="10" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A67" s="12" t="s">
         <v>235</v>
       </c>
-      <c r="B67" s="15"/>
+      <c r="B67" s="15" t="s">
+        <v>551</v>
+      </c>
       <c r="C67" s="9" t="s">
         <v>287</v>
       </c>
@@ -6442,19 +6487,45 @@
       <c r="E67" s="9" t="s">
         <v>289</v>
       </c>
-      <c r="F67" s="9"/>
-      <c r="G67" s="9"/>
-      <c r="H67" s="9"/>
-      <c r="I67" s="9"/>
-      <c r="J67" s="9"/>
-      <c r="K67" s="9"/>
-      <c r="L67" s="9"/>
-      <c r="M67" s="9"/>
-      <c r="N67" s="9"/>
-      <c r="O67" s="9"/>
-      <c r="P67" s="9"/>
-      <c r="Q67" s="9"/>
-      <c r="R67" s="9"/>
+      <c r="F67" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="G67" s="9" t="s">
+        <v>320</v>
+      </c>
+      <c r="H67" s="9" t="s">
+        <v>336</v>
+      </c>
+      <c r="I67" s="9" t="s">
+        <v>351</v>
+      </c>
+      <c r="J67" s="9" t="s">
+        <v>329</v>
+      </c>
+      <c r="K67" s="9" t="s">
+        <v>554</v>
+      </c>
+      <c r="L67" s="9" t="s">
+        <v>553</v>
+      </c>
+      <c r="M67" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="N67" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="O67" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="P67" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="Q67" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="R67" s="10" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A68" s="12" t="s">

</xml_diff>

<commit_message>
feat: implement STA ind, ADC abs,X, and ADC abs,Y instructions
</commit_message>
<xml_diff>
--- a/docs/PandesalCPU Specs.xlsx
+++ b/docs/PandesalCPU Specs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shim Manaloto\Documents\PandesalCPU\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E963BAC0-11EC-45CF-B3B3-C3897E975D69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F689302A-0118-4D7C-9DFC-E05FB85C198B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{A2A5A835-37AC-4F29-881C-332D1F6F724B}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1585" uniqueCount="555">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1627" uniqueCount="559">
   <si>
     <t>000</t>
   </si>
@@ -1699,10 +1699,22 @@
     <t>0101 0110 000 1 1 01 0</t>
   </si>
   <si>
-    <t>0000 000 000 0 0 01 1</t>
-  </si>
-  <si>
     <t>0101 1111 000 1 1 00 0</t>
+  </si>
+  <si>
+    <t>0000 0000 000 0 0 01 1</t>
+  </si>
+  <si>
+    <t>STA ind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1111 0001 000 0 1 00 0 </t>
+  </si>
+  <si>
+    <t>ADC abs,X</t>
+  </si>
+  <si>
+    <t>ADC abs,Y</t>
   </si>
 </sst>
 </file>
@@ -2270,10 +2282,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E48F8AD-971A-4094-8D85-72B0AE25E8BF}">
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:K38"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="114" workbookViewId="0">
-      <selection activeCell="G6" sqref="A1:G6"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2680,6 +2692,50 @@
         <v>111</v>
       </c>
     </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+    </row>
+    <row r="35" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+    </row>
+    <row r="36" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+    </row>
+    <row r="37" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+    </row>
+    <row r="38" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2694,8 +2750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC51F965-835D-4E82-9AC8-2752CA30592B}">
   <dimension ref="A1:AJ257"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H54" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L67" sqref="L67"/>
+    <sheetView tabSelected="1" topLeftCell="I57" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="J70" sqref="J70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6503,10 +6559,10 @@
         <v>329</v>
       </c>
       <c r="K67" s="9" t="s">
+        <v>553</v>
+      </c>
+      <c r="L67" s="9" t="s">
         <v>554</v>
-      </c>
-      <c r="L67" s="9" t="s">
-        <v>553</v>
       </c>
       <c r="M67" s="10" t="s">
         <v>305</v>
@@ -6531,7 +6587,9 @@
       <c r="A68" s="12" t="s">
         <v>242</v>
       </c>
-      <c r="B68" s="15"/>
+      <c r="B68" s="15" t="s">
+        <v>555</v>
+      </c>
       <c r="C68" s="9" t="s">
         <v>287</v>
       </c>
@@ -6541,25 +6599,53 @@
       <c r="E68" s="9" t="s">
         <v>289</v>
       </c>
-      <c r="F68" s="9"/>
-      <c r="G68" s="9"/>
-      <c r="H68" s="9"/>
-      <c r="I68" s="9"/>
-      <c r="J68" s="9"/>
-      <c r="K68" s="9"/>
-      <c r="L68" s="9"/>
-      <c r="M68" s="9"/>
-      <c r="N68" s="9"/>
-      <c r="O68" s="9"/>
-      <c r="P68" s="9"/>
-      <c r="Q68" s="9"/>
-      <c r="R68" s="8"/>
+      <c r="F68" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="G68" s="9" t="s">
+        <v>320</v>
+      </c>
+      <c r="H68" s="9" t="s">
+        <v>336</v>
+      </c>
+      <c r="I68" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="J68" s="9" t="s">
+        <v>556</v>
+      </c>
+      <c r="K68" s="9" t="s">
+        <v>336</v>
+      </c>
+      <c r="L68" s="9" t="s">
+        <v>337</v>
+      </c>
+      <c r="M68" s="9" t="s">
+        <v>554</v>
+      </c>
+      <c r="N68" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="O68" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="P68" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="Q68" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="R68" s="10" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="69" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A69" s="12" t="s">
         <v>243</v>
       </c>
-      <c r="B69" s="15"/>
+      <c r="B69" s="15" t="s">
+        <v>557</v>
+      </c>
       <c r="C69" s="9" t="s">
         <v>287</v>
       </c>
@@ -6569,25 +6655,53 @@
       <c r="E69" s="9" t="s">
         <v>289</v>
       </c>
-      <c r="F69" s="9"/>
-      <c r="G69" s="9"/>
-      <c r="H69" s="9"/>
-      <c r="I69" s="9"/>
-      <c r="J69" s="9"/>
-      <c r="K69" s="9"/>
-      <c r="L69" s="9"/>
-      <c r="M69" s="9"/>
-      <c r="N69" s="9"/>
-      <c r="O69" s="9"/>
-      <c r="P69" s="9"/>
-      <c r="Q69" s="9"/>
-      <c r="R69" s="8"/>
+      <c r="F69" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="G69" s="9" t="s">
+        <v>320</v>
+      </c>
+      <c r="H69" s="9" t="s">
+        <v>336</v>
+      </c>
+      <c r="I69" s="9" t="s">
+        <v>368</v>
+      </c>
+      <c r="J69" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="K69" s="9" t="s">
+        <v>359</v>
+      </c>
+      <c r="L69" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="M69" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="N69" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="O69" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="P69" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="Q69" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="R69" s="10" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="70" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A70" s="12" t="s">
         <v>244</v>
       </c>
-      <c r="B70" s="15"/>
+      <c r="B70" s="15" t="s">
+        <v>558</v>
+      </c>
       <c r="C70" s="9" t="s">
         <v>287</v>
       </c>
@@ -6597,19 +6711,45 @@
       <c r="E70" s="9" t="s">
         <v>289</v>
       </c>
-      <c r="F70" s="9"/>
-      <c r="G70" s="9"/>
-      <c r="H70" s="9"/>
-      <c r="I70" s="9"/>
-      <c r="J70" s="9"/>
-      <c r="K70" s="9"/>
-      <c r="L70" s="9"/>
-      <c r="M70" s="9"/>
-      <c r="N70" s="9"/>
-      <c r="O70" s="9"/>
-      <c r="P70" s="9"/>
-      <c r="Q70" s="9"/>
-      <c r="R70" s="8"/>
+      <c r="F70" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="G70" s="9" t="s">
+        <v>320</v>
+      </c>
+      <c r="H70" s="9" t="s">
+        <v>336</v>
+      </c>
+      <c r="I70" s="9" t="s">
+        <v>545</v>
+      </c>
+      <c r="J70" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="K70" s="9" t="s">
+        <v>359</v>
+      </c>
+      <c r="L70" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="M70" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="N70" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="O70" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="P70" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="Q70" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="R70" s="10" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="71" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A71" s="12" t="s">

</xml_diff>

<commit_message>
feat: implement ADD # and SUB # instructions
</commit_message>
<xml_diff>
--- a/docs/PandesalCPU Specs.xlsx
+++ b/docs/PandesalCPU Specs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shim Manaloto\Documents\PandesalCPU\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F689302A-0118-4D7C-9DFC-E05FB85C198B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C49AFB13-AD2B-462E-B631-B5117E808C43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{A2A5A835-37AC-4F29-881C-332D1F6F724B}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1627" uniqueCount="559">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1655" uniqueCount="563">
   <si>
     <t>000</t>
   </si>
@@ -1715,6 +1715,18 @@
   </si>
   <si>
     <t>ADC abs,Y</t>
+  </si>
+  <si>
+    <t>ADD #</t>
+  </si>
+  <si>
+    <t>SUB #</t>
+  </si>
+  <si>
+    <t>0101 0110 000 1 1 01 1</t>
+  </si>
+  <si>
+    <t>0101 0110 001 1 1 01 1</t>
   </si>
 </sst>
 </file>
@@ -2750,8 +2762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC51F965-835D-4E82-9AC8-2752CA30592B}">
   <dimension ref="A1:AJ257"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I57" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J70" sqref="J70"/>
+    <sheetView tabSelected="1" topLeftCell="E62" zoomScale="125" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H71" sqref="H71:R72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6755,7 +6767,9 @@
       <c r="A71" s="12" t="s">
         <v>245</v>
       </c>
-      <c r="B71" s="15"/>
+      <c r="B71" s="15" t="s">
+        <v>559</v>
+      </c>
       <c r="C71" s="9" t="s">
         <v>287</v>
       </c>
@@ -6765,25 +6779,53 @@
       <c r="E71" s="9" t="s">
         <v>289</v>
       </c>
-      <c r="F71" s="9"/>
-      <c r="G71" s="9"/>
-      <c r="H71" s="9"/>
-      <c r="I71" s="9"/>
-      <c r="J71" s="9"/>
-      <c r="K71" s="9"/>
-      <c r="L71" s="9"/>
-      <c r="M71" s="9"/>
-      <c r="N71" s="9"/>
-      <c r="O71" s="9"/>
-      <c r="P71" s="9"/>
-      <c r="Q71" s="9"/>
-      <c r="R71" s="8"/>
+      <c r="F71" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="G71" s="9" t="s">
+        <v>561</v>
+      </c>
+      <c r="H71" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="I71" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="J71" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="K71" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="L71" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="M71" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="N71" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="O71" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="P71" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="Q71" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="R71" s="10" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="72" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A72" s="12" t="s">
         <v>246</v>
       </c>
-      <c r="B72" s="15"/>
+      <c r="B72" s="15" t="s">
+        <v>560</v>
+      </c>
       <c r="C72" s="9" t="s">
         <v>287</v>
       </c>
@@ -6793,19 +6835,45 @@
       <c r="E72" s="9" t="s">
         <v>289</v>
       </c>
-      <c r="F72" s="9"/>
-      <c r="G72" s="9"/>
-      <c r="H72" s="9"/>
-      <c r="I72" s="9"/>
-      <c r="J72" s="9"/>
-      <c r="K72" s="9"/>
-      <c r="L72" s="9"/>
-      <c r="M72" s="9"/>
-      <c r="N72" s="9"/>
-      <c r="O72" s="9"/>
-      <c r="P72" s="9"/>
-      <c r="Q72" s="9"/>
-      <c r="R72" s="8"/>
+      <c r="F72" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="G72" s="9" t="s">
+        <v>562</v>
+      </c>
+      <c r="H72" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="I72" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="J72" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="K72" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="L72" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="M72" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="N72" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="O72" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="P72" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="Q72" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="R72" s="10" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="73" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A73" s="12" t="s">

</xml_diff>

<commit_message>
feat: implement ADD abs and SUB abs instructions
</commit_message>
<xml_diff>
--- a/docs/PandesalCPU Specs.xlsx
+++ b/docs/PandesalCPU Specs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shim Manaloto\Documents\PandesalCPU\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C49AFB13-AD2B-462E-B631-B5117E808C43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC6BC6DB-F382-4100-923B-C5CE021FEB92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{A2A5A835-37AC-4F29-881C-332D1F6F724B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{A2A5A835-37AC-4F29-881C-332D1F6F724B}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1655" uniqueCount="563">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1683" uniqueCount="566">
   <si>
     <t>000</t>
   </si>
@@ -1727,6 +1727,15 @@
   </si>
   <si>
     <t>0101 0110 001 1 1 01 1</t>
+  </si>
+  <si>
+    <t>ADD abs</t>
+  </si>
+  <si>
+    <t>SUB abs</t>
+  </si>
+  <si>
+    <t>0101 0110 001 1 1 01 0</t>
   </si>
 </sst>
 </file>
@@ -2762,8 +2771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC51F965-835D-4E82-9AC8-2752CA30592B}">
   <dimension ref="A1:AJ257"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E62" zoomScale="125" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H71" sqref="H71:R72"/>
+    <sheetView tabSelected="1" topLeftCell="E63" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25:H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6879,7 +6888,9 @@
       <c r="A73" s="12" t="s">
         <v>247</v>
       </c>
-      <c r="B73" s="15"/>
+      <c r="B73" s="15" t="s">
+        <v>563</v>
+      </c>
       <c r="C73" s="9" t="s">
         <v>287</v>
       </c>
@@ -6889,25 +6900,53 @@
       <c r="E73" s="9" t="s">
         <v>289</v>
       </c>
-      <c r="F73" s="9"/>
-      <c r="G73" s="9"/>
-      <c r="H73" s="9"/>
-      <c r="I73" s="9"/>
-      <c r="J73" s="9"/>
-      <c r="K73" s="9"/>
-      <c r="L73" s="9"/>
-      <c r="M73" s="9"/>
-      <c r="N73" s="9"/>
-      <c r="O73" s="9"/>
-      <c r="P73" s="9"/>
-      <c r="Q73" s="9"/>
-      <c r="R73" s="8"/>
+      <c r="F73" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="G73" s="9" t="s">
+        <v>320</v>
+      </c>
+      <c r="H73" s="9" t="s">
+        <v>336</v>
+      </c>
+      <c r="I73" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="J73" s="9" t="s">
+        <v>305</v>
+      </c>
+      <c r="K73" s="9" t="s">
+        <v>552</v>
+      </c>
+      <c r="L73" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="M73" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="N73" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="O73" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="P73" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="Q73" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="R73" s="10" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="74" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A74" s="12" t="s">
         <v>248</v>
       </c>
-      <c r="B74" s="15"/>
+      <c r="B74" s="15" t="s">
+        <v>564</v>
+      </c>
       <c r="C74" s="9" t="s">
         <v>287</v>
       </c>
@@ -6917,19 +6956,45 @@
       <c r="E74" s="9" t="s">
         <v>289</v>
       </c>
-      <c r="F74" s="9"/>
-      <c r="G74" s="9"/>
-      <c r="H74" s="9"/>
-      <c r="I74" s="9"/>
-      <c r="J74" s="9"/>
-      <c r="K74" s="9"/>
-      <c r="L74" s="9"/>
-      <c r="M74" s="9"/>
-      <c r="N74" s="9"/>
-      <c r="O74" s="9"/>
-      <c r="P74" s="9"/>
-      <c r="Q74" s="9"/>
-      <c r="R74" s="8"/>
+      <c r="F74" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="G74" s="9" t="s">
+        <v>320</v>
+      </c>
+      <c r="H74" s="9" t="s">
+        <v>336</v>
+      </c>
+      <c r="I74" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="J74" s="9" t="s">
+        <v>305</v>
+      </c>
+      <c r="K74" s="9" t="s">
+        <v>565</v>
+      </c>
+      <c r="L74" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="M74" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="N74" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="O74" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="P74" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="Q74" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="R74" s="10" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="75" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A75" s="12" t="s">

</xml_diff>

<commit_message>
fix: correct RTS implementation to increment at the end
</commit_message>
<xml_diff>
--- a/docs/PandesalCPU Specs.xlsx
+++ b/docs/PandesalCPU Specs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shim Manaloto\Documents\PandesalCPU\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{148CB30D-66C2-47FB-BAD8-8FE3A5AF71B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA34751-F403-48F1-9F14-B82687875D97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{A2A5A835-37AC-4F29-881C-332D1F6F724B}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1683" uniqueCount="566">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1683" uniqueCount="567">
   <si>
     <t>000</t>
   </si>
@@ -1135,9 +1135,6 @@
     <t>0000 1111 000 0 0 00 0</t>
   </si>
   <si>
-    <t>1111 0000 000 0 1 01 1</t>
-  </si>
-  <si>
     <t>1000 0110 001 1 1 00 0</t>
   </si>
   <si>
@@ -1736,6 +1733,12 @@
   </si>
   <si>
     <t>CMP #</t>
+  </si>
+  <si>
+    <t>1111 0000 000 0 1 00 1</t>
+  </si>
+  <si>
+    <t>0111  0111 000 0 0 01 1</t>
   </si>
 </sst>
 </file>
@@ -2305,7 +2308,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E48F8AD-971A-4094-8D85-72B0AE25E8BF}">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="114" workbookViewId="0">
+    <sheetView zoomScale="114" workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
@@ -2771,8 +2774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC51F965-835D-4E82-9AC8-2752CA30592B}">
   <dimension ref="A1:AJ257"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="109" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4184,7 +4187,7 @@
         <v>364</v>
       </c>
       <c r="O24" s="9" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="P24" s="9" t="s">
         <v>355</v>
@@ -4461,10 +4464,10 @@
         <v>363</v>
       </c>
       <c r="N29" s="19" t="s">
-        <v>365</v>
-      </c>
-      <c r="O29" s="10" t="s">
-        <v>304</v>
+        <v>565</v>
+      </c>
+      <c r="O29" s="19" t="s">
+        <v>566</v>
       </c>
       <c r="P29" s="10" t="s">
         <v>304</v>
@@ -5321,7 +5324,7 @@
         <v>208</v>
       </c>
       <c r="B45" s="15" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C45" s="9" t="s">
         <v>286</v>
@@ -6182,7 +6185,7 @@
         <v>335</v>
       </c>
       <c r="I60" s="9" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="J60" s="9" t="s">
         <v>290</v>
@@ -6238,7 +6241,7 @@
         <v>335</v>
       </c>
       <c r="I61" s="9" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="J61" s="9" t="s">
         <v>290</v>
@@ -6294,13 +6297,13 @@
         <v>335</v>
       </c>
       <c r="I62" s="9" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="J62" s="9" t="s">
         <v>291</v>
       </c>
       <c r="K62" s="9" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="L62" s="10" t="s">
         <v>304</v>
@@ -6350,13 +6353,13 @@
         <v>335</v>
       </c>
       <c r="I63" s="9" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="J63" s="9" t="s">
         <v>291</v>
       </c>
       <c r="K63" s="9" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="L63" s="10" t="s">
         <v>304</v>
@@ -6406,7 +6409,7 @@
         <v>335</v>
       </c>
       <c r="I64" s="9" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="J64" s="9" t="s">
         <v>304</v>
@@ -6462,7 +6465,7 @@
         <v>335</v>
       </c>
       <c r="I65" s="9" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="J65" s="9" t="s">
         <v>304</v>
@@ -6497,7 +6500,7 @@
         <v>234</v>
       </c>
       <c r="B66" s="15" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C66" s="9" t="s">
         <v>286</v>
@@ -6512,7 +6515,7 @@
         <v>328</v>
       </c>
       <c r="G66" s="9" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H66" s="10" t="s">
         <v>304</v>
@@ -6553,7 +6556,7 @@
         <v>235</v>
       </c>
       <c r="B67" s="15" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C67" s="9" t="s">
         <v>286</v>
@@ -6580,10 +6583,10 @@
         <v>328</v>
       </c>
       <c r="K67" s="9" t="s">
+        <v>551</v>
+      </c>
+      <c r="L67" s="9" t="s">
         <v>552</v>
-      </c>
-      <c r="L67" s="9" t="s">
-        <v>553</v>
       </c>
       <c r="M67" s="10" t="s">
         <v>304</v>
@@ -6609,7 +6612,7 @@
         <v>242</v>
       </c>
       <c r="B68" s="15" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="C68" s="9" t="s">
         <v>286</v>
@@ -6633,7 +6636,7 @@
         <v>291</v>
       </c>
       <c r="J68" s="9" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="K68" s="9" t="s">
         <v>335</v>
@@ -6642,7 +6645,7 @@
         <v>336</v>
       </c>
       <c r="M68" s="9" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="N68" s="10" t="s">
         <v>304</v>
@@ -6665,7 +6668,7 @@
         <v>243</v>
       </c>
       <c r="B69" s="15" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C69" s="9" t="s">
         <v>286</v>
@@ -6686,7 +6689,7 @@
         <v>335</v>
       </c>
       <c r="I69" s="9" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="J69" s="9" t="s">
         <v>291</v>
@@ -6721,7 +6724,7 @@
         <v>244</v>
       </c>
       <c r="B70" s="15" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="C70" s="9" t="s">
         <v>286</v>
@@ -6742,7 +6745,7 @@
         <v>335</v>
       </c>
       <c r="I70" s="9" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="J70" s="9" t="s">
         <v>291</v>
@@ -6777,7 +6780,7 @@
         <v>245</v>
       </c>
       <c r="B71" s="15" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C71" s="9" t="s">
         <v>286</v>
@@ -6792,7 +6795,7 @@
         <v>292</v>
       </c>
       <c r="G71" s="9" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="H71" s="10" t="s">
         <v>304</v>
@@ -6833,7 +6836,7 @@
         <v>246</v>
       </c>
       <c r="B72" s="15" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C72" s="9" t="s">
         <v>286</v>
@@ -6848,7 +6851,7 @@
         <v>292</v>
       </c>
       <c r="G72" s="9" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="H72" s="10" t="s">
         <v>304</v>
@@ -6889,7 +6892,7 @@
         <v>247</v>
       </c>
       <c r="B73" s="15" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C73" s="9" t="s">
         <v>286</v>
@@ -6916,7 +6919,7 @@
         <v>304</v>
       </c>
       <c r="K73" s="9" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="L73" s="10" t="s">
         <v>304</v>
@@ -6945,7 +6948,7 @@
         <v>248</v>
       </c>
       <c r="B74" s="15" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="C74" s="9" t="s">
         <v>286</v>
@@ -6972,7 +6975,7 @@
         <v>304</v>
       </c>
       <c r="K74" s="9" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="L74" s="10" t="s">
         <v>304</v>
@@ -7182,7 +7185,7 @@
     </row>
     <row r="82" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A82" s="12" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B82" s="15"/>
       <c r="C82" s="9"/>
@@ -7204,7 +7207,7 @@
     </row>
     <row r="83" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A83" s="12" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B83" s="15"/>
       <c r="C83" s="9"/>
@@ -7226,7 +7229,7 @@
     </row>
     <row r="84" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A84" s="12" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B84" s="15"/>
       <c r="C84" s="9"/>
@@ -7248,7 +7251,7 @@
     </row>
     <row r="85" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A85" s="12" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B85" s="15"/>
       <c r="C85" s="9"/>
@@ -7270,7 +7273,7 @@
     </row>
     <row r="86" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A86" s="12" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B86" s="15"/>
       <c r="C86" s="9"/>
@@ -7292,7 +7295,7 @@
     </row>
     <row r="87" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A87" s="12" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B87" s="14"/>
       <c r="C87" s="8"/>
@@ -7314,7 +7317,7 @@
     </row>
     <row r="88" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A88" s="12" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B88" s="14"/>
       <c r="C88" s="8"/>
@@ -7336,7 +7339,7 @@
     </row>
     <row r="89" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A89" s="12" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B89" s="14"/>
       <c r="C89" s="8"/>
@@ -7358,7 +7361,7 @@
     </row>
     <row r="90" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A90" s="12" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B90" s="14"/>
       <c r="C90" s="8"/>
@@ -7380,7 +7383,7 @@
     </row>
     <row r="91" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A91" s="12" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B91" s="14"/>
       <c r="C91" s="8"/>
@@ -7402,7 +7405,7 @@
     </row>
     <row r="92" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A92" s="12" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B92" s="14"/>
       <c r="C92" s="8"/>
@@ -7424,7 +7427,7 @@
     </row>
     <row r="93" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A93" s="12" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B93" s="14"/>
       <c r="C93" s="8"/>
@@ -7446,7 +7449,7 @@
     </row>
     <row r="94" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A94" s="12" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B94" s="14"/>
       <c r="C94" s="8"/>
@@ -7468,7 +7471,7 @@
     </row>
     <row r="95" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A95" s="12" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B95" s="14"/>
       <c r="C95" s="8"/>
@@ -7490,7 +7493,7 @@
     </row>
     <row r="96" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A96" s="12" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B96" s="14"/>
       <c r="C96" s="8"/>
@@ -7512,7 +7515,7 @@
     </row>
     <row r="97" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A97" s="12" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B97" s="14"/>
       <c r="C97" s="8"/>
@@ -7534,7 +7537,7 @@
     </row>
     <row r="98" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A98" s="12" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B98" s="14"/>
       <c r="C98" s="8"/>
@@ -7556,7 +7559,7 @@
     </row>
     <row r="99" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A99" s="12" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B99" s="14"/>
       <c r="C99" s="8"/>
@@ -7578,7 +7581,7 @@
     </row>
     <row r="100" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A100" s="12" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B100" s="14"/>
       <c r="C100" s="8"/>
@@ -7600,7 +7603,7 @@
     </row>
     <row r="101" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A101" s="12" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B101" s="14"/>
       <c r="C101" s="8"/>
@@ -7622,7 +7625,7 @@
     </row>
     <row r="102" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A102" s="12" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B102" s="14"/>
       <c r="C102" s="8"/>
@@ -7644,7 +7647,7 @@
     </row>
     <row r="103" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A103" s="12" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B103" s="14"/>
       <c r="C103" s="8"/>
@@ -7666,7 +7669,7 @@
     </row>
     <row r="104" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A104" s="12" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B104" s="14"/>
       <c r="C104" s="8"/>
@@ -7688,7 +7691,7 @@
     </row>
     <row r="105" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A105" s="12" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B105" s="14"/>
       <c r="C105" s="8"/>
@@ -7710,7 +7713,7 @@
     </row>
     <row r="106" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A106" s="12" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B106" s="14"/>
       <c r="C106" s="8"/>
@@ -7732,7 +7735,7 @@
     </row>
     <row r="107" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A107" s="12" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B107" s="14"/>
       <c r="C107" s="8"/>
@@ -7754,7 +7757,7 @@
     </row>
     <row r="108" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A108" s="12" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B108" s="14"/>
       <c r="C108" s="8"/>
@@ -7776,7 +7779,7 @@
     </row>
     <row r="109" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A109" s="12" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B109" s="14"/>
       <c r="C109" s="8"/>
@@ -7798,7 +7801,7 @@
     </row>
     <row r="110" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A110" s="12" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B110" s="14"/>
       <c r="C110" s="8"/>
@@ -7820,7 +7823,7 @@
     </row>
     <row r="111" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A111" s="12" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B111" s="14"/>
       <c r="C111" s="8"/>
@@ -7842,7 +7845,7 @@
     </row>
     <row r="112" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A112" s="12" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B112" s="14"/>
       <c r="C112" s="8"/>
@@ -7864,7 +7867,7 @@
     </row>
     <row r="113" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A113" s="12" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B113" s="14"/>
       <c r="C113" s="8"/>
@@ -7886,7 +7889,7 @@
     </row>
     <row r="114" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A114" s="12" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B114" s="14"/>
       <c r="C114" s="8"/>
@@ -7908,7 +7911,7 @@
     </row>
     <row r="115" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A115" s="12" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B115" s="14"/>
       <c r="C115" s="8"/>
@@ -7930,7 +7933,7 @@
     </row>
     <row r="116" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A116" s="12" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B116" s="14"/>
       <c r="C116" s="8"/>
@@ -7952,7 +7955,7 @@
     </row>
     <row r="117" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A117" s="12" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B117" s="14"/>
       <c r="C117" s="8"/>
@@ -7974,7 +7977,7 @@
     </row>
     <row r="118" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A118" s="12" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B118" s="14"/>
       <c r="C118" s="8"/>
@@ -7996,7 +7999,7 @@
     </row>
     <row r="119" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A119" s="12" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B119" s="14"/>
       <c r="C119" s="8"/>
@@ -8018,7 +8021,7 @@
     </row>
     <row r="120" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A120" s="12" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B120" s="14"/>
       <c r="C120" s="8"/>
@@ -8040,7 +8043,7 @@
     </row>
     <row r="121" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A121" s="12" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B121" s="14"/>
       <c r="C121" s="8"/>
@@ -8062,7 +8065,7 @@
     </row>
     <row r="122" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A122" s="12" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B122" s="14"/>
       <c r="C122" s="8"/>
@@ -8084,7 +8087,7 @@
     </row>
     <row r="123" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A123" s="12" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B123" s="14"/>
       <c r="C123" s="8"/>
@@ -8106,7 +8109,7 @@
     </row>
     <row r="124" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A124" s="12" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B124" s="14"/>
       <c r="C124" s="8"/>
@@ -8128,7 +8131,7 @@
     </row>
     <row r="125" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A125" s="12" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B125" s="14"/>
       <c r="C125" s="8"/>
@@ -8150,7 +8153,7 @@
     </row>
     <row r="126" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A126" s="12" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B126" s="14"/>
       <c r="C126" s="8"/>
@@ -8172,7 +8175,7 @@
     </row>
     <row r="127" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A127" s="12" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B127" s="14"/>
       <c r="C127" s="8"/>
@@ -8194,7 +8197,7 @@
     </row>
     <row r="128" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A128" s="12" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B128" s="14"/>
       <c r="C128" s="8"/>
@@ -8216,7 +8219,7 @@
     </row>
     <row r="129" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A129" s="12" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B129" s="14"/>
       <c r="C129" s="8"/>
@@ -8238,7 +8241,7 @@
     </row>
     <row r="130" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A130" s="12" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B130" s="14"/>
       <c r="C130" s="8"/>
@@ -8260,7 +8263,7 @@
     </row>
     <row r="131" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A131" s="12" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B131" s="14"/>
       <c r="C131" s="8"/>
@@ -8282,7 +8285,7 @@
     </row>
     <row r="132" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A132" s="12" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B132" s="14"/>
       <c r="C132" s="8"/>
@@ -8304,7 +8307,7 @@
     </row>
     <row r="133" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A133" s="12" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B133" s="14"/>
       <c r="C133" s="8"/>
@@ -8326,7 +8329,7 @@
     </row>
     <row r="134" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A134" s="12" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B134" s="14"/>
       <c r="C134" s="8"/>
@@ -8348,7 +8351,7 @@
     </row>
     <row r="135" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A135" s="12" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B135" s="14"/>
       <c r="C135" s="8"/>
@@ -8370,7 +8373,7 @@
     </row>
     <row r="136" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A136" s="12" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B136" s="14"/>
       <c r="C136" s="8"/>
@@ -8392,7 +8395,7 @@
     </row>
     <row r="137" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A137" s="12" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B137" s="14"/>
       <c r="C137" s="8"/>
@@ -8414,7 +8417,7 @@
     </row>
     <row r="138" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A138" s="12" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B138" s="14"/>
       <c r="C138" s="8"/>
@@ -8436,7 +8439,7 @@
     </row>
     <row r="139" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A139" s="12" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B139" s="14"/>
       <c r="C139" s="8"/>
@@ -8458,7 +8461,7 @@
     </row>
     <row r="140" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A140" s="12" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B140" s="14"/>
       <c r="C140" s="8"/>
@@ -8480,7 +8483,7 @@
     </row>
     <row r="141" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A141" s="12" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B141" s="14"/>
       <c r="C141" s="8"/>
@@ -8502,7 +8505,7 @@
     </row>
     <row r="142" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A142" s="12" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B142" s="14"/>
       <c r="C142" s="8"/>
@@ -8524,7 +8527,7 @@
     </row>
     <row r="143" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A143" s="12" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B143" s="14"/>
       <c r="C143" s="8"/>
@@ -8546,7 +8549,7 @@
     </row>
     <row r="144" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A144" s="12" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B144" s="14"/>
       <c r="C144" s="8"/>
@@ -8568,7 +8571,7 @@
     </row>
     <row r="145" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A145" s="12" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B145" s="14"/>
       <c r="C145" s="8"/>
@@ -8590,7 +8593,7 @@
     </row>
     <row r="146" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A146" s="12" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B146" s="14"/>
       <c r="C146" s="8"/>
@@ -8612,7 +8615,7 @@
     </row>
     <row r="147" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A147" s="12" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B147" s="14"/>
       <c r="C147" s="8"/>
@@ -8634,7 +8637,7 @@
     </row>
     <row r="148" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A148" s="12" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B148" s="14"/>
       <c r="C148" s="8"/>
@@ -8656,7 +8659,7 @@
     </row>
     <row r="149" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A149" s="12" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B149" s="14"/>
       <c r="C149" s="8"/>
@@ -8678,7 +8681,7 @@
     </row>
     <row r="150" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A150" s="12" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B150" s="14"/>
       <c r="C150" s="8"/>
@@ -8700,7 +8703,7 @@
     </row>
     <row r="151" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A151" s="12" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B151" s="14"/>
       <c r="C151" s="8"/>
@@ -8722,7 +8725,7 @@
     </row>
     <row r="152" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A152" s="12" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B152" s="14"/>
       <c r="C152" s="8"/>
@@ -8744,7 +8747,7 @@
     </row>
     <row r="153" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A153" s="12" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B153" s="14"/>
       <c r="C153" s="8"/>
@@ -8766,7 +8769,7 @@
     </row>
     <row r="154" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A154" s="12" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B154" s="14"/>
       <c r="C154" s="8"/>
@@ -8788,7 +8791,7 @@
     </row>
     <row r="155" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A155" s="12" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B155" s="14"/>
       <c r="C155" s="8"/>
@@ -8810,7 +8813,7 @@
     </row>
     <row r="156" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A156" s="12" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B156" s="14"/>
       <c r="C156" s="8"/>
@@ -8832,7 +8835,7 @@
     </row>
     <row r="157" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A157" s="12" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B157" s="14"/>
       <c r="C157" s="8"/>
@@ -8854,7 +8857,7 @@
     </row>
     <row r="158" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A158" s="12" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B158" s="14"/>
       <c r="C158" s="8"/>
@@ -8876,7 +8879,7 @@
     </row>
     <row r="159" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A159" s="12" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B159" s="14"/>
       <c r="C159" s="8"/>
@@ -8898,7 +8901,7 @@
     </row>
     <row r="160" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A160" s="12" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B160" s="14"/>
       <c r="C160" s="8"/>
@@ -8920,7 +8923,7 @@
     </row>
     <row r="161" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A161" s="12" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B161" s="14"/>
       <c r="C161" s="8"/>
@@ -8942,7 +8945,7 @@
     </row>
     <row r="162" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A162" s="12" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B162" s="14"/>
       <c r="C162" s="8"/>
@@ -8964,7 +8967,7 @@
     </row>
     <row r="163" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A163" s="12" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B163" s="14"/>
       <c r="C163" s="8"/>
@@ -8986,7 +8989,7 @@
     </row>
     <row r="164" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A164" s="12" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B164" s="14"/>
       <c r="C164" s="8"/>
@@ -9008,7 +9011,7 @@
     </row>
     <row r="165" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A165" s="12" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B165" s="14"/>
       <c r="C165" s="8"/>
@@ -9030,7 +9033,7 @@
     </row>
     <row r="166" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A166" s="12" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B166" s="14"/>
       <c r="C166" s="8"/>
@@ -9052,7 +9055,7 @@
     </row>
     <row r="167" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A167" s="12" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B167" s="14"/>
       <c r="C167" s="8"/>
@@ -9074,7 +9077,7 @@
     </row>
     <row r="168" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A168" s="12" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B168" s="14"/>
       <c r="C168" s="8"/>
@@ -9096,7 +9099,7 @@
     </row>
     <row r="169" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A169" s="12" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B169" s="14"/>
       <c r="C169" s="8"/>
@@ -9118,7 +9121,7 @@
     </row>
     <row r="170" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A170" s="12" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B170" s="14"/>
       <c r="C170" s="8"/>
@@ -9140,7 +9143,7 @@
     </row>
     <row r="171" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A171" s="12" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B171" s="14"/>
       <c r="C171" s="8"/>
@@ -9162,7 +9165,7 @@
     </row>
     <row r="172" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A172" s="12" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B172" s="14"/>
       <c r="C172" s="8"/>
@@ -9184,7 +9187,7 @@
     </row>
     <row r="173" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A173" s="12" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B173" s="14"/>
       <c r="C173" s="8"/>
@@ -9206,7 +9209,7 @@
     </row>
     <row r="174" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A174" s="12" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B174" s="14"/>
       <c r="C174" s="8"/>
@@ -9228,7 +9231,7 @@
     </row>
     <row r="175" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A175" s="12" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B175" s="14"/>
       <c r="C175" s="8"/>
@@ -9250,7 +9253,7 @@
     </row>
     <row r="176" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A176" s="12" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B176" s="14"/>
       <c r="C176" s="8"/>
@@ -9272,7 +9275,7 @@
     </row>
     <row r="177" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A177" s="12" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B177" s="14"/>
       <c r="C177" s="8"/>
@@ -9294,7 +9297,7 @@
     </row>
     <row r="178" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A178" s="12" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B178" s="14"/>
       <c r="C178" s="8"/>
@@ -9316,7 +9319,7 @@
     </row>
     <row r="179" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A179" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B179" s="14"/>
       <c r="C179" s="8"/>
@@ -9338,7 +9341,7 @@
     </row>
     <row r="180" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A180" s="12" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B180" s="14"/>
       <c r="C180" s="8"/>
@@ -9360,7 +9363,7 @@
     </row>
     <row r="181" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A181" s="12" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B181" s="14"/>
       <c r="C181" s="8"/>
@@ -9382,7 +9385,7 @@
     </row>
     <row r="182" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A182" s="12" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B182" s="14"/>
       <c r="C182" s="8"/>
@@ -9404,7 +9407,7 @@
     </row>
     <row r="183" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A183" s="12" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B183" s="14"/>
       <c r="C183" s="8"/>
@@ -9426,7 +9429,7 @@
     </row>
     <row r="184" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A184" s="12" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B184" s="14"/>
       <c r="C184" s="8"/>
@@ -9448,7 +9451,7 @@
     </row>
     <row r="185" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A185" s="12" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B185" s="14"/>
       <c r="C185" s="8"/>
@@ -9470,7 +9473,7 @@
     </row>
     <row r="186" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A186" s="12" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B186" s="14"/>
       <c r="C186" s="8"/>
@@ -9492,7 +9495,7 @@
     </row>
     <row r="187" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A187" s="12" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B187" s="14"/>
       <c r="C187" s="8"/>
@@ -9514,7 +9517,7 @@
     </row>
     <row r="188" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A188" s="12" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B188" s="14"/>
       <c r="C188" s="8"/>
@@ -9536,7 +9539,7 @@
     </row>
     <row r="189" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A189" s="12" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B189" s="14"/>
       <c r="C189" s="8"/>
@@ -9558,7 +9561,7 @@
     </row>
     <row r="190" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A190" s="12" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B190" s="14"/>
       <c r="C190" s="8"/>
@@ -9580,7 +9583,7 @@
     </row>
     <row r="191" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A191" s="12" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B191" s="14"/>
       <c r="C191" s="8"/>
@@ -9602,7 +9605,7 @@
     </row>
     <row r="192" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A192" s="12" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B192" s="14"/>
       <c r="C192" s="8"/>
@@ -9624,7 +9627,7 @@
     </row>
     <row r="193" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A193" s="12" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B193" s="14"/>
       <c r="C193" s="8"/>
@@ -9646,7 +9649,7 @@
     </row>
     <row r="194" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A194" s="12" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B194" s="14"/>
       <c r="C194" s="8"/>
@@ -9668,7 +9671,7 @@
     </row>
     <row r="195" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A195" s="12" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B195" s="14"/>
       <c r="C195" s="8"/>
@@ -9690,7 +9693,7 @@
     </row>
     <row r="196" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A196" s="12" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B196" s="14"/>
       <c r="C196" s="8"/>
@@ -9712,7 +9715,7 @@
     </row>
     <row r="197" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A197" s="12" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B197" s="14"/>
       <c r="C197" s="8"/>
@@ -9734,7 +9737,7 @@
     </row>
     <row r="198" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A198" s="12" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B198" s="14"/>
       <c r="C198" s="8"/>
@@ -9756,7 +9759,7 @@
     </row>
     <row r="199" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A199" s="12" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B199" s="14"/>
       <c r="C199" s="8"/>
@@ -9778,7 +9781,7 @@
     </row>
     <row r="200" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A200" s="12" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B200" s="14"/>
       <c r="C200" s="8"/>
@@ -9800,7 +9803,7 @@
     </row>
     <row r="201" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A201" s="12" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B201" s="14"/>
       <c r="C201" s="8"/>
@@ -9822,7 +9825,7 @@
     </row>
     <row r="202" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A202" s="12" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B202" s="14"/>
       <c r="C202" s="8"/>
@@ -9844,7 +9847,7 @@
     </row>
     <row r="203" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A203" s="12" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B203" s="14"/>
       <c r="C203" s="8"/>
@@ -9866,7 +9869,7 @@
     </row>
     <row r="204" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A204" s="12" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B204" s="14"/>
       <c r="C204" s="8"/>
@@ -9888,7 +9891,7 @@
     </row>
     <row r="205" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A205" s="12" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B205" s="14"/>
       <c r="C205" s="8"/>
@@ -9910,7 +9913,7 @@
     </row>
     <row r="206" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A206" s="12" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B206" s="14"/>
       <c r="C206" s="8"/>
@@ -9932,7 +9935,7 @@
     </row>
     <row r="207" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A207" s="12" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B207" s="14"/>
       <c r="C207" s="8"/>
@@ -9954,7 +9957,7 @@
     </row>
     <row r="208" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A208" s="12" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B208" s="14"/>
       <c r="C208" s="8"/>
@@ -9976,7 +9979,7 @@
     </row>
     <row r="209" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A209" s="12" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B209" s="14"/>
       <c r="C209" s="8"/>
@@ -9998,7 +10001,7 @@
     </row>
     <row r="210" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A210" s="12" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B210" s="14"/>
       <c r="C210" s="8"/>
@@ -10020,7 +10023,7 @@
     </row>
     <row r="211" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A211" s="12" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B211" s="14"/>
       <c r="C211" s="8"/>
@@ -10042,7 +10045,7 @@
     </row>
     <row r="212" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A212" s="12" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B212" s="14"/>
       <c r="C212" s="8"/>
@@ -10064,7 +10067,7 @@
     </row>
     <row r="213" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A213" s="12" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B213" s="14"/>
       <c r="C213" s="8"/>
@@ -10086,7 +10089,7 @@
     </row>
     <row r="214" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A214" s="12" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B214" s="14"/>
       <c r="C214" s="8"/>
@@ -10108,7 +10111,7 @@
     </row>
     <row r="215" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A215" s="12" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B215" s="14"/>
       <c r="C215" s="8"/>
@@ -10130,7 +10133,7 @@
     </row>
     <row r="216" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A216" s="12" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B216" s="14"/>
       <c r="C216" s="8"/>
@@ -10152,7 +10155,7 @@
     </row>
     <row r="217" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A217" s="12" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B217" s="14"/>
       <c r="C217" s="8"/>
@@ -10174,7 +10177,7 @@
     </row>
     <row r="218" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A218" s="12" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B218" s="14"/>
       <c r="C218" s="8"/>
@@ -10196,7 +10199,7 @@
     </row>
     <row r="219" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A219" s="12" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B219" s="14"/>
       <c r="C219" s="8"/>
@@ -10218,7 +10221,7 @@
     </row>
     <row r="220" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A220" s="12" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B220" s="14"/>
       <c r="C220" s="8"/>
@@ -10240,7 +10243,7 @@
     </row>
     <row r="221" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A221" s="12" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B221" s="14"/>
       <c r="C221" s="8"/>
@@ -10262,7 +10265,7 @@
     </row>
     <row r="222" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A222" s="12" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B222" s="14"/>
       <c r="C222" s="8"/>
@@ -10284,7 +10287,7 @@
     </row>
     <row r="223" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A223" s="12" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B223" s="14"/>
       <c r="C223" s="8"/>
@@ -10306,7 +10309,7 @@
     </row>
     <row r="224" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A224" s="12" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B224" s="14"/>
       <c r="C224" s="8"/>
@@ -10328,7 +10331,7 @@
     </row>
     <row r="225" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A225" s="12" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B225" s="14"/>
       <c r="C225" s="8"/>
@@ -10350,7 +10353,7 @@
     </row>
     <row r="226" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A226" s="12" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B226" s="14"/>
       <c r="C226" s="8"/>
@@ -10372,7 +10375,7 @@
     </row>
     <row r="227" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A227" s="12" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B227" s="14"/>
       <c r="C227" s="8"/>
@@ -10394,7 +10397,7 @@
     </row>
     <row r="228" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A228" s="12" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B228" s="14"/>
       <c r="C228" s="8"/>
@@ -10416,7 +10419,7 @@
     </row>
     <row r="229" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A229" s="12" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B229" s="14"/>
       <c r="C229" s="8"/>
@@ -10438,7 +10441,7 @@
     </row>
     <row r="230" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A230" s="12" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B230" s="14"/>
       <c r="C230" s="8"/>
@@ -10460,7 +10463,7 @@
     </row>
     <row r="231" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A231" s="12" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B231" s="14"/>
       <c r="C231" s="8"/>
@@ -10482,7 +10485,7 @@
     </row>
     <row r="232" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A232" s="12" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B232" s="14"/>
       <c r="C232" s="8"/>
@@ -10504,7 +10507,7 @@
     </row>
     <row r="233" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A233" s="12" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B233" s="14"/>
       <c r="C233" s="8"/>
@@ -10526,7 +10529,7 @@
     </row>
     <row r="234" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A234" s="12" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B234" s="14"/>
       <c r="C234" s="8"/>
@@ -10548,7 +10551,7 @@
     </row>
     <row r="235" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A235" s="12" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B235" s="14"/>
       <c r="C235" s="8"/>
@@ -10570,7 +10573,7 @@
     </row>
     <row r="236" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A236" s="12" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B236" s="14"/>
       <c r="C236" s="8"/>
@@ -10592,7 +10595,7 @@
     </row>
     <row r="237" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A237" s="12" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B237" s="14"/>
       <c r="C237" s="8"/>
@@ -10614,7 +10617,7 @@
     </row>
     <row r="238" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A238" s="12" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B238" s="14"/>
       <c r="C238" s="8"/>
@@ -10636,7 +10639,7 @@
     </row>
     <row r="239" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A239" s="12" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B239" s="14"/>
       <c r="C239" s="8"/>
@@ -10658,7 +10661,7 @@
     </row>
     <row r="240" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A240" s="12" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B240" s="14"/>
       <c r="C240" s="8"/>
@@ -10680,7 +10683,7 @@
     </row>
     <row r="241" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A241" s="12" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B241" s="14"/>
       <c r="C241" s="8"/>
@@ -10702,7 +10705,7 @@
     </row>
     <row r="242" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A242" s="12" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B242" s="14"/>
       <c r="C242" s="8"/>
@@ -10724,7 +10727,7 @@
     </row>
     <row r="243" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A243" s="12" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B243" s="14"/>
       <c r="C243" s="8"/>
@@ -10746,7 +10749,7 @@
     </row>
     <row r="244" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A244" s="12" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B244" s="14"/>
       <c r="C244" s="8"/>
@@ -10768,7 +10771,7 @@
     </row>
     <row r="245" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A245" s="12" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B245" s="14"/>
       <c r="C245" s="8"/>
@@ -10790,7 +10793,7 @@
     </row>
     <row r="246" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A246" s="12" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B246" s="14"/>
       <c r="C246" s="8"/>
@@ -10812,7 +10815,7 @@
     </row>
     <row r="247" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A247" s="12" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B247" s="14"/>
       <c r="C247" s="8"/>
@@ -10834,7 +10837,7 @@
     </row>
     <row r="248" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A248" s="12" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B248" s="14"/>
       <c r="C248" s="8"/>
@@ -10856,7 +10859,7 @@
     </row>
     <row r="249" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A249" s="12" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B249" s="14"/>
       <c r="C249" s="8"/>
@@ -10878,7 +10881,7 @@
     </row>
     <row r="250" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A250" s="12" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B250" s="14"/>
       <c r="C250" s="8"/>
@@ -10900,7 +10903,7 @@
     </row>
     <row r="251" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A251" s="12" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B251" s="14"/>
       <c r="C251" s="8"/>
@@ -10922,7 +10925,7 @@
     </row>
     <row r="252" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A252" s="12" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B252" s="14"/>
       <c r="C252" s="8"/>
@@ -10944,7 +10947,7 @@
     </row>
     <row r="253" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A253" s="12" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B253" s="14"/>
       <c r="C253" s="8"/>
@@ -10966,7 +10969,7 @@
     </row>
     <row r="254" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A254" s="12" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B254" s="14"/>
       <c r="C254" s="8"/>
@@ -10988,7 +10991,7 @@
     </row>
     <row r="255" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A255" s="12" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B255" s="14"/>
       <c r="C255" s="8"/>
@@ -11010,7 +11013,7 @@
     </row>
     <row r="256" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A256" s="12" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B256" s="14"/>
       <c r="C256" s="8"/>
@@ -11032,7 +11035,7 @@
     </row>
     <row r="257" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A257" s="12" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B257" s="14"/>
       <c r="C257" s="8"/>
@@ -11117,7 +11120,7 @@
         <v>19</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C2" s="22"/>
       <c r="D2" s="22"/>

</xml_diff>

<commit_message>
fix: correct STX abs and STY abs implementation by incrementing at the last cycle
</commit_message>
<xml_diff>
--- a/docs/PandesalCPU Specs.xlsx
+++ b/docs/PandesalCPU Specs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shim Manaloto\Documents\PandesalCPU\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA34751-F403-48F1-9F14-B82687875D97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB83CD54-C28F-44B3-B16A-2F0686DE1791}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{A2A5A835-37AC-4F29-881C-332D1F6F724B}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1683" uniqueCount="567">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1683" uniqueCount="566">
   <si>
     <t>000</t>
   </si>
@@ -1084,12 +1084,6 @@
     <t>0110 1111 000 0 0 01 0</t>
   </si>
   <si>
-    <t>1001 1111 000 0 0 01 0</t>
-  </si>
-  <si>
-    <t>1010 1111 000 0 0 01 0</t>
-  </si>
-  <si>
     <t>1111 0110 000 0 0 00 0</t>
   </si>
   <si>
@@ -1738,7 +1732,10 @@
     <t>1111 0000 000 0 1 00 1</t>
   </si>
   <si>
-    <t>0111  0111 000 0 0 01 1</t>
+    <t>1001 1111 000 0 0 00 0</t>
+  </si>
+  <si>
+    <t>1010 1111 000 0 0 00 0</t>
   </si>
 </sst>
 </file>
@@ -2774,8 +2771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC51F965-835D-4E82-9AC8-2752CA30592B}">
   <dimension ref="A1:AJ257"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="109" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3665,10 +3662,10 @@
         <v>335</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>348</v>
-      </c>
-      <c r="J15" s="10" t="s">
-        <v>304</v>
+        <v>564</v>
+      </c>
+      <c r="J15" s="9" t="s">
+        <v>360</v>
       </c>
       <c r="K15" s="10" t="s">
         <v>304</v>
@@ -3721,10 +3718,10 @@
         <v>335</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>349</v>
-      </c>
-      <c r="J16" s="10" t="s">
-        <v>304</v>
+        <v>565</v>
+      </c>
+      <c r="J16" s="9" t="s">
+        <v>360</v>
       </c>
       <c r="K16" s="10" t="s">
         <v>304</v>
@@ -4063,7 +4060,7 @@
         <v>328</v>
       </c>
       <c r="K22" s="9" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="L22" s="10" t="s">
         <v>304</v>
@@ -4119,7 +4116,7 @@
         <v>327</v>
       </c>
       <c r="K23" s="9" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="L23" s="10" t="s">
         <v>304</v>
@@ -4175,7 +4172,7 @@
         <v>328</v>
       </c>
       <c r="K24" s="9" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="L24" s="9" t="s">
         <v>301</v>
@@ -4184,13 +4181,13 @@
         <v>304</v>
       </c>
       <c r="N24" s="9" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="O24" s="9" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="P24" s="9" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="Q24" s="10" t="s">
         <v>304</v>
@@ -4399,7 +4396,7 @@
         <v>304</v>
       </c>
       <c r="K28" s="9" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="L28" s="10" t="s">
         <v>304</v>
@@ -4455,19 +4452,19 @@
         <v>327</v>
       </c>
       <c r="K29" s="18" t="s">
+        <v>357</v>
+      </c>
+      <c r="L29" s="19" t="s">
         <v>359</v>
       </c>
-      <c r="L29" s="19" t="s">
+      <c r="M29" s="19" t="s">
         <v>361</v>
       </c>
-      <c r="M29" s="19" t="s">
-        <v>363</v>
-      </c>
       <c r="N29" s="19" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="O29" s="19" t="s">
-        <v>566</v>
+        <v>360</v>
       </c>
       <c r="P29" s="10" t="s">
         <v>304</v>
@@ -4511,7 +4508,7 @@
         <v>304</v>
       </c>
       <c r="K30" s="9" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="L30" s="10" t="s">
         <v>304</v>
@@ -5324,7 +5321,7 @@
         <v>208</v>
       </c>
       <c r="B45" s="15" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="C45" s="9" t="s">
         <v>286</v>
@@ -5625,16 +5622,16 @@
         <v>335</v>
       </c>
       <c r="I50" s="9" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="J50" s="9" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="K50" s="9" t="s">
         <v>336</v>
       </c>
       <c r="L50" s="9" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="M50" s="10" t="s">
         <v>304</v>
@@ -5681,16 +5678,16 @@
         <v>335</v>
       </c>
       <c r="I51" s="9" t="s">
+        <v>348</v>
+      </c>
+      <c r="J51" s="9" t="s">
         <v>350</v>
-      </c>
-      <c r="J51" s="9" t="s">
-        <v>352</v>
       </c>
       <c r="K51" s="9" t="s">
         <v>336</v>
       </c>
       <c r="L51" s="9" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="M51" s="10" t="s">
         <v>304</v>
@@ -5737,16 +5734,16 @@
         <v>335</v>
       </c>
       <c r="I52" s="9" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="J52" s="9" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="K52" s="9" t="s">
         <v>336</v>
       </c>
       <c r="L52" s="9" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="M52" s="10" t="s">
         <v>304</v>
@@ -5793,16 +5790,16 @@
         <v>335</v>
       </c>
       <c r="I53" s="9" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="J53" s="9" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="K53" s="9" t="s">
         <v>336</v>
       </c>
       <c r="L53" s="9" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="M53" s="10" t="s">
         <v>304</v>
@@ -6185,7 +6182,7 @@
         <v>335</v>
       </c>
       <c r="I60" s="9" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="J60" s="9" t="s">
         <v>290</v>
@@ -6241,7 +6238,7 @@
         <v>335</v>
       </c>
       <c r="I61" s="9" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="J61" s="9" t="s">
         <v>290</v>
@@ -6297,13 +6294,13 @@
         <v>335</v>
       </c>
       <c r="I62" s="9" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="J62" s="9" t="s">
         <v>291</v>
       </c>
       <c r="K62" s="9" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="L62" s="10" t="s">
         <v>304</v>
@@ -6353,13 +6350,13 @@
         <v>335</v>
       </c>
       <c r="I63" s="9" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="J63" s="9" t="s">
         <v>291</v>
       </c>
       <c r="K63" s="9" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="L63" s="10" t="s">
         <v>304</v>
@@ -6409,7 +6406,7 @@
         <v>335</v>
       </c>
       <c r="I64" s="9" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="J64" s="9" t="s">
         <v>304</v>
@@ -6465,7 +6462,7 @@
         <v>335</v>
       </c>
       <c r="I65" s="9" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="J65" s="9" t="s">
         <v>304</v>
@@ -6500,7 +6497,7 @@
         <v>234</v>
       </c>
       <c r="B66" s="15" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="C66" s="9" t="s">
         <v>286</v>
@@ -6515,7 +6512,7 @@
         <v>328</v>
       </c>
       <c r="G66" s="9" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="H66" s="10" t="s">
         <v>304</v>
@@ -6556,7 +6553,7 @@
         <v>235</v>
       </c>
       <c r="B67" s="15" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C67" s="9" t="s">
         <v>286</v>
@@ -6577,16 +6574,16 @@
         <v>335</v>
       </c>
       <c r="I67" s="9" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="J67" s="9" t="s">
         <v>328</v>
       </c>
       <c r="K67" s="9" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="L67" s="9" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="M67" s="10" t="s">
         <v>304</v>
@@ -6612,7 +6609,7 @@
         <v>242</v>
       </c>
       <c r="B68" s="15" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C68" s="9" t="s">
         <v>286</v>
@@ -6636,7 +6633,7 @@
         <v>291</v>
       </c>
       <c r="J68" s="9" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="K68" s="9" t="s">
         <v>335</v>
@@ -6645,7 +6642,7 @@
         <v>336</v>
       </c>
       <c r="M68" s="9" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="N68" s="10" t="s">
         <v>304</v>
@@ -6668,7 +6665,7 @@
         <v>243</v>
       </c>
       <c r="B69" s="15" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="C69" s="9" t="s">
         <v>286</v>
@@ -6689,13 +6686,13 @@
         <v>335</v>
       </c>
       <c r="I69" s="9" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="J69" s="9" t="s">
         <v>291</v>
       </c>
       <c r="K69" s="9" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="L69" s="10" t="s">
         <v>304</v>
@@ -6724,7 +6721,7 @@
         <v>244</v>
       </c>
       <c r="B70" s="15" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="C70" s="9" t="s">
         <v>286</v>
@@ -6745,13 +6742,13 @@
         <v>335</v>
       </c>
       <c r="I70" s="9" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="J70" s="9" t="s">
         <v>291</v>
       </c>
       <c r="K70" s="9" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="L70" s="10" t="s">
         <v>304</v>
@@ -6780,7 +6777,7 @@
         <v>245</v>
       </c>
       <c r="B71" s="15" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="C71" s="9" t="s">
         <v>286</v>
@@ -6795,7 +6792,7 @@
         <v>292</v>
       </c>
       <c r="G71" s="9" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="H71" s="10" t="s">
         <v>304</v>
@@ -6836,7 +6833,7 @@
         <v>246</v>
       </c>
       <c r="B72" s="15" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="C72" s="9" t="s">
         <v>286</v>
@@ -6851,7 +6848,7 @@
         <v>292</v>
       </c>
       <c r="G72" s="9" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="H72" s="10" t="s">
         <v>304</v>
@@ -6892,7 +6889,7 @@
         <v>247</v>
       </c>
       <c r="B73" s="15" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="C73" s="9" t="s">
         <v>286</v>
@@ -6919,7 +6916,7 @@
         <v>304</v>
       </c>
       <c r="K73" s="9" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="L73" s="10" t="s">
         <v>304</v>
@@ -6948,7 +6945,7 @@
         <v>248</v>
       </c>
       <c r="B74" s="15" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="C74" s="9" t="s">
         <v>286</v>
@@ -6975,7 +6972,7 @@
         <v>304</v>
       </c>
       <c r="K74" s="9" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="L74" s="10" t="s">
         <v>304</v>
@@ -7185,7 +7182,7 @@
     </row>
     <row r="82" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A82" s="12" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B82" s="15"/>
       <c r="C82" s="9"/>
@@ -7207,7 +7204,7 @@
     </row>
     <row r="83" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A83" s="12" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B83" s="15"/>
       <c r="C83" s="9"/>
@@ -7229,7 +7226,7 @@
     </row>
     <row r="84" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A84" s="12" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B84" s="15"/>
       <c r="C84" s="9"/>
@@ -7251,7 +7248,7 @@
     </row>
     <row r="85" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A85" s="12" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B85" s="15"/>
       <c r="C85" s="9"/>
@@ -7273,7 +7270,7 @@
     </row>
     <row r="86" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A86" s="12" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B86" s="15"/>
       <c r="C86" s="9"/>
@@ -7295,7 +7292,7 @@
     </row>
     <row r="87" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A87" s="12" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B87" s="14"/>
       <c r="C87" s="8"/>
@@ -7317,7 +7314,7 @@
     </row>
     <row r="88" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A88" s="12" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B88" s="14"/>
       <c r="C88" s="8"/>
@@ -7339,7 +7336,7 @@
     </row>
     <row r="89" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A89" s="12" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B89" s="14"/>
       <c r="C89" s="8"/>
@@ -7361,7 +7358,7 @@
     </row>
     <row r="90" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A90" s="12" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B90" s="14"/>
       <c r="C90" s="8"/>
@@ -7383,7 +7380,7 @@
     </row>
     <row r="91" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A91" s="12" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B91" s="14"/>
       <c r="C91" s="8"/>
@@ -7405,7 +7402,7 @@
     </row>
     <row r="92" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A92" s="12" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B92" s="14"/>
       <c r="C92" s="8"/>
@@ -7427,7 +7424,7 @@
     </row>
     <row r="93" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A93" s="12" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B93" s="14"/>
       <c r="C93" s="8"/>
@@ -7449,7 +7446,7 @@
     </row>
     <row r="94" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A94" s="12" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B94" s="14"/>
       <c r="C94" s="8"/>
@@ -7471,7 +7468,7 @@
     </row>
     <row r="95" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A95" s="12" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B95" s="14"/>
       <c r="C95" s="8"/>
@@ -7493,7 +7490,7 @@
     </row>
     <row r="96" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A96" s="12" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B96" s="14"/>
       <c r="C96" s="8"/>
@@ -7515,7 +7512,7 @@
     </row>
     <row r="97" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A97" s="12" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B97" s="14"/>
       <c r="C97" s="8"/>
@@ -7537,7 +7534,7 @@
     </row>
     <row r="98" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A98" s="12" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B98" s="14"/>
       <c r="C98" s="8"/>
@@ -7559,7 +7556,7 @@
     </row>
     <row r="99" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A99" s="12" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B99" s="14"/>
       <c r="C99" s="8"/>
@@ -7581,7 +7578,7 @@
     </row>
     <row r="100" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A100" s="12" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B100" s="14"/>
       <c r="C100" s="8"/>
@@ -7603,7 +7600,7 @@
     </row>
     <row r="101" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A101" s="12" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B101" s="14"/>
       <c r="C101" s="8"/>
@@ -7625,7 +7622,7 @@
     </row>
     <row r="102" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A102" s="12" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B102" s="14"/>
       <c r="C102" s="8"/>
@@ -7647,7 +7644,7 @@
     </row>
     <row r="103" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A103" s="12" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B103" s="14"/>
       <c r="C103" s="8"/>
@@ -7669,7 +7666,7 @@
     </row>
     <row r="104" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A104" s="12" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B104" s="14"/>
       <c r="C104" s="8"/>
@@ -7691,7 +7688,7 @@
     </row>
     <row r="105" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A105" s="12" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B105" s="14"/>
       <c r="C105" s="8"/>
@@ -7713,7 +7710,7 @@
     </row>
     <row r="106" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A106" s="12" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B106" s="14"/>
       <c r="C106" s="8"/>
@@ -7735,7 +7732,7 @@
     </row>
     <row r="107" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A107" s="12" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B107" s="14"/>
       <c r="C107" s="8"/>
@@ -7757,7 +7754,7 @@
     </row>
     <row r="108" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A108" s="12" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B108" s="14"/>
       <c r="C108" s="8"/>
@@ -7779,7 +7776,7 @@
     </row>
     <row r="109" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A109" s="12" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B109" s="14"/>
       <c r="C109" s="8"/>
@@ -7801,7 +7798,7 @@
     </row>
     <row r="110" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A110" s="12" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B110" s="14"/>
       <c r="C110" s="8"/>
@@ -7823,7 +7820,7 @@
     </row>
     <row r="111" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A111" s="12" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B111" s="14"/>
       <c r="C111" s="8"/>
@@ -7845,7 +7842,7 @@
     </row>
     <row r="112" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A112" s="12" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B112" s="14"/>
       <c r="C112" s="8"/>
@@ -7867,7 +7864,7 @@
     </row>
     <row r="113" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A113" s="12" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B113" s="14"/>
       <c r="C113" s="8"/>
@@ -7889,7 +7886,7 @@
     </row>
     <row r="114" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A114" s="12" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B114" s="14"/>
       <c r="C114" s="8"/>
@@ -7911,7 +7908,7 @@
     </row>
     <row r="115" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A115" s="12" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B115" s="14"/>
       <c r="C115" s="8"/>
@@ -7933,7 +7930,7 @@
     </row>
     <row r="116" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A116" s="12" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B116" s="14"/>
       <c r="C116" s="8"/>
@@ -7955,7 +7952,7 @@
     </row>
     <row r="117" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A117" s="12" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B117" s="14"/>
       <c r="C117" s="8"/>
@@ -7977,7 +7974,7 @@
     </row>
     <row r="118" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A118" s="12" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B118" s="14"/>
       <c r="C118" s="8"/>
@@ -7999,7 +7996,7 @@
     </row>
     <row r="119" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A119" s="12" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B119" s="14"/>
       <c r="C119" s="8"/>
@@ -8021,7 +8018,7 @@
     </row>
     <row r="120" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A120" s="12" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B120" s="14"/>
       <c r="C120" s="8"/>
@@ -8043,7 +8040,7 @@
     </row>
     <row r="121" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A121" s="12" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B121" s="14"/>
       <c r="C121" s="8"/>
@@ -8065,7 +8062,7 @@
     </row>
     <row r="122" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A122" s="12" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B122" s="14"/>
       <c r="C122" s="8"/>
@@ -8087,7 +8084,7 @@
     </row>
     <row r="123" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A123" s="12" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B123" s="14"/>
       <c r="C123" s="8"/>
@@ -8109,7 +8106,7 @@
     </row>
     <row r="124" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A124" s="12" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B124" s="14"/>
       <c r="C124" s="8"/>
@@ -8131,7 +8128,7 @@
     </row>
     <row r="125" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A125" s="12" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B125" s="14"/>
       <c r="C125" s="8"/>
@@ -8153,7 +8150,7 @@
     </row>
     <row r="126" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A126" s="12" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B126" s="14"/>
       <c r="C126" s="8"/>
@@ -8175,7 +8172,7 @@
     </row>
     <row r="127" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A127" s="12" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B127" s="14"/>
       <c r="C127" s="8"/>
@@ -8197,7 +8194,7 @@
     </row>
     <row r="128" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A128" s="12" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B128" s="14"/>
       <c r="C128" s="8"/>
@@ -8219,7 +8216,7 @@
     </row>
     <row r="129" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A129" s="12" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B129" s="14"/>
       <c r="C129" s="8"/>
@@ -8241,7 +8238,7 @@
     </row>
     <row r="130" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A130" s="12" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B130" s="14"/>
       <c r="C130" s="8"/>
@@ -8263,7 +8260,7 @@
     </row>
     <row r="131" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A131" s="12" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B131" s="14"/>
       <c r="C131" s="8"/>
@@ -8285,7 +8282,7 @@
     </row>
     <row r="132" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A132" s="12" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B132" s="14"/>
       <c r="C132" s="8"/>
@@ -8307,7 +8304,7 @@
     </row>
     <row r="133" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A133" s="12" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B133" s="14"/>
       <c r="C133" s="8"/>
@@ -8329,7 +8326,7 @@
     </row>
     <row r="134" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A134" s="12" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B134" s="14"/>
       <c r="C134" s="8"/>
@@ -8351,7 +8348,7 @@
     </row>
     <row r="135" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A135" s="12" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B135" s="14"/>
       <c r="C135" s="8"/>
@@ -8373,7 +8370,7 @@
     </row>
     <row r="136" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A136" s="12" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B136" s="14"/>
       <c r="C136" s="8"/>
@@ -8395,7 +8392,7 @@
     </row>
     <row r="137" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A137" s="12" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B137" s="14"/>
       <c r="C137" s="8"/>
@@ -8417,7 +8414,7 @@
     </row>
     <row r="138" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A138" s="12" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B138" s="14"/>
       <c r="C138" s="8"/>
@@ -8439,7 +8436,7 @@
     </row>
     <row r="139" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A139" s="12" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B139" s="14"/>
       <c r="C139" s="8"/>
@@ -8461,7 +8458,7 @@
     </row>
     <row r="140" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A140" s="12" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B140" s="14"/>
       <c r="C140" s="8"/>
@@ -8483,7 +8480,7 @@
     </row>
     <row r="141" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A141" s="12" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B141" s="14"/>
       <c r="C141" s="8"/>
@@ -8505,7 +8502,7 @@
     </row>
     <row r="142" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A142" s="12" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B142" s="14"/>
       <c r="C142" s="8"/>
@@ -8527,7 +8524,7 @@
     </row>
     <row r="143" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A143" s="12" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B143" s="14"/>
       <c r="C143" s="8"/>
@@ -8549,7 +8546,7 @@
     </row>
     <row r="144" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A144" s="12" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B144" s="14"/>
       <c r="C144" s="8"/>
@@ -8571,7 +8568,7 @@
     </row>
     <row r="145" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A145" s="12" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B145" s="14"/>
       <c r="C145" s="8"/>
@@ -8593,7 +8590,7 @@
     </row>
     <row r="146" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A146" s="12" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B146" s="14"/>
       <c r="C146" s="8"/>
@@ -8615,7 +8612,7 @@
     </row>
     <row r="147" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A147" s="12" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B147" s="14"/>
       <c r="C147" s="8"/>
@@ -8637,7 +8634,7 @@
     </row>
     <row r="148" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A148" s="12" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="B148" s="14"/>
       <c r="C148" s="8"/>
@@ -8659,7 +8656,7 @@
     </row>
     <row r="149" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A149" s="12" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B149" s="14"/>
       <c r="C149" s="8"/>
@@ -8681,7 +8678,7 @@
     </row>
     <row r="150" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A150" s="12" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B150" s="14"/>
       <c r="C150" s="8"/>
@@ -8703,7 +8700,7 @@
     </row>
     <row r="151" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A151" s="12" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B151" s="14"/>
       <c r="C151" s="8"/>
@@ -8725,7 +8722,7 @@
     </row>
     <row r="152" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A152" s="12" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B152" s="14"/>
       <c r="C152" s="8"/>
@@ -8747,7 +8744,7 @@
     </row>
     <row r="153" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A153" s="12" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B153" s="14"/>
       <c r="C153" s="8"/>
@@ -8769,7 +8766,7 @@
     </row>
     <row r="154" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A154" s="12" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B154" s="14"/>
       <c r="C154" s="8"/>
@@ -8791,7 +8788,7 @@
     </row>
     <row r="155" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A155" s="12" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B155" s="14"/>
       <c r="C155" s="8"/>
@@ -8813,7 +8810,7 @@
     </row>
     <row r="156" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A156" s="12" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="B156" s="14"/>
       <c r="C156" s="8"/>
@@ -8835,7 +8832,7 @@
     </row>
     <row r="157" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A157" s="12" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B157" s="14"/>
       <c r="C157" s="8"/>
@@ -8857,7 +8854,7 @@
     </row>
     <row r="158" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A158" s="12" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B158" s="14"/>
       <c r="C158" s="8"/>
@@ -8879,7 +8876,7 @@
     </row>
     <row r="159" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A159" s="12" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B159" s="14"/>
       <c r="C159" s="8"/>
@@ -8901,7 +8898,7 @@
     </row>
     <row r="160" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A160" s="12" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B160" s="14"/>
       <c r="C160" s="8"/>
@@ -8923,7 +8920,7 @@
     </row>
     <row r="161" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A161" s="12" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B161" s="14"/>
       <c r="C161" s="8"/>
@@ -8945,7 +8942,7 @@
     </row>
     <row r="162" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A162" s="12" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B162" s="14"/>
       <c r="C162" s="8"/>
@@ -8967,7 +8964,7 @@
     </row>
     <row r="163" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A163" s="12" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B163" s="14"/>
       <c r="C163" s="8"/>
@@ -8989,7 +8986,7 @@
     </row>
     <row r="164" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A164" s="12" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B164" s="14"/>
       <c r="C164" s="8"/>
@@ -9011,7 +9008,7 @@
     </row>
     <row r="165" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A165" s="12" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B165" s="14"/>
       <c r="C165" s="8"/>
@@ -9033,7 +9030,7 @@
     </row>
     <row r="166" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A166" s="12" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="B166" s="14"/>
       <c r="C166" s="8"/>
@@ -9055,7 +9052,7 @@
     </row>
     <row r="167" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A167" s="12" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B167" s="14"/>
       <c r="C167" s="8"/>
@@ -9077,7 +9074,7 @@
     </row>
     <row r="168" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A168" s="12" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B168" s="14"/>
       <c r="C168" s="8"/>
@@ -9099,7 +9096,7 @@
     </row>
     <row r="169" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A169" s="12" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="B169" s="14"/>
       <c r="C169" s="8"/>
@@ -9121,7 +9118,7 @@
     </row>
     <row r="170" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A170" s="12" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="B170" s="14"/>
       <c r="C170" s="8"/>
@@ -9143,7 +9140,7 @@
     </row>
     <row r="171" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A171" s="12" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B171" s="14"/>
       <c r="C171" s="8"/>
@@ -9165,7 +9162,7 @@
     </row>
     <row r="172" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A172" s="12" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="B172" s="14"/>
       <c r="C172" s="8"/>
@@ -9187,7 +9184,7 @@
     </row>
     <row r="173" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A173" s="12" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="B173" s="14"/>
       <c r="C173" s="8"/>
@@ -9209,7 +9206,7 @@
     </row>
     <row r="174" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A174" s="12" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="B174" s="14"/>
       <c r="C174" s="8"/>
@@ -9231,7 +9228,7 @@
     </row>
     <row r="175" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A175" s="12" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="B175" s="14"/>
       <c r="C175" s="8"/>
@@ -9253,7 +9250,7 @@
     </row>
     <row r="176" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A176" s="12" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="B176" s="14"/>
       <c r="C176" s="8"/>
@@ -9275,7 +9272,7 @@
     </row>
     <row r="177" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A177" s="12" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B177" s="14"/>
       <c r="C177" s="8"/>
@@ -9297,7 +9294,7 @@
     </row>
     <row r="178" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A178" s="12" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B178" s="14"/>
       <c r="C178" s="8"/>
@@ -9319,7 +9316,7 @@
     </row>
     <row r="179" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A179" s="12" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="B179" s="14"/>
       <c r="C179" s="8"/>
@@ -9341,7 +9338,7 @@
     </row>
     <row r="180" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A180" s="12" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="B180" s="14"/>
       <c r="C180" s="8"/>
@@ -9363,7 +9360,7 @@
     </row>
     <row r="181" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A181" s="12" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="B181" s="14"/>
       <c r="C181" s="8"/>
@@ -9385,7 +9382,7 @@
     </row>
     <row r="182" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A182" s="12" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B182" s="14"/>
       <c r="C182" s="8"/>
@@ -9407,7 +9404,7 @@
     </row>
     <row r="183" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A183" s="12" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="B183" s="14"/>
       <c r="C183" s="8"/>
@@ -9429,7 +9426,7 @@
     </row>
     <row r="184" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A184" s="12" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="B184" s="14"/>
       <c r="C184" s="8"/>
@@ -9451,7 +9448,7 @@
     </row>
     <row r="185" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A185" s="12" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="B185" s="14"/>
       <c r="C185" s="8"/>
@@ -9473,7 +9470,7 @@
     </row>
     <row r="186" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A186" s="12" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B186" s="14"/>
       <c r="C186" s="8"/>
@@ -9495,7 +9492,7 @@
     </row>
     <row r="187" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A187" s="12" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B187" s="14"/>
       <c r="C187" s="8"/>
@@ -9517,7 +9514,7 @@
     </row>
     <row r="188" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A188" s="12" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B188" s="14"/>
       <c r="C188" s="8"/>
@@ -9539,7 +9536,7 @@
     </row>
     <row r="189" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A189" s="12" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B189" s="14"/>
       <c r="C189" s="8"/>
@@ -9561,7 +9558,7 @@
     </row>
     <row r="190" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A190" s="12" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B190" s="14"/>
       <c r="C190" s="8"/>
@@ -9583,7 +9580,7 @@
     </row>
     <row r="191" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A191" s="12" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B191" s="14"/>
       <c r="C191" s="8"/>
@@ -9605,7 +9602,7 @@
     </row>
     <row r="192" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A192" s="12" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B192" s="14"/>
       <c r="C192" s="8"/>
@@ -9627,7 +9624,7 @@
     </row>
     <row r="193" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A193" s="12" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="B193" s="14"/>
       <c r="C193" s="8"/>
@@ -9649,7 +9646,7 @@
     </row>
     <row r="194" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A194" s="12" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="B194" s="14"/>
       <c r="C194" s="8"/>
@@ -9671,7 +9668,7 @@
     </row>
     <row r="195" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A195" s="12" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="B195" s="14"/>
       <c r="C195" s="8"/>
@@ -9693,7 +9690,7 @@
     </row>
     <row r="196" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A196" s="12" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B196" s="14"/>
       <c r="C196" s="8"/>
@@ -9715,7 +9712,7 @@
     </row>
     <row r="197" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A197" s="12" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="B197" s="14"/>
       <c r="C197" s="8"/>
@@ -9737,7 +9734,7 @@
     </row>
     <row r="198" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A198" s="12" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="B198" s="14"/>
       <c r="C198" s="8"/>
@@ -9759,7 +9756,7 @@
     </row>
     <row r="199" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A199" s="12" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="B199" s="14"/>
       <c r="C199" s="8"/>
@@ -9781,7 +9778,7 @@
     </row>
     <row r="200" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A200" s="12" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B200" s="14"/>
       <c r="C200" s="8"/>
@@ -9803,7 +9800,7 @@
     </row>
     <row r="201" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A201" s="12" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B201" s="14"/>
       <c r="C201" s="8"/>
@@ -9825,7 +9822,7 @@
     </row>
     <row r="202" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A202" s="12" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B202" s="14"/>
       <c r="C202" s="8"/>
@@ -9847,7 +9844,7 @@
     </row>
     <row r="203" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A203" s="12" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="B203" s="14"/>
       <c r="C203" s="8"/>
@@ -9869,7 +9866,7 @@
     </row>
     <row r="204" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A204" s="12" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="B204" s="14"/>
       <c r="C204" s="8"/>
@@ -9891,7 +9888,7 @@
     </row>
     <row r="205" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A205" s="12" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="B205" s="14"/>
       <c r="C205" s="8"/>
@@ -9913,7 +9910,7 @@
     </row>
     <row r="206" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A206" s="12" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="B206" s="14"/>
       <c r="C206" s="8"/>
@@ -9935,7 +9932,7 @@
     </row>
     <row r="207" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A207" s="12" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B207" s="14"/>
       <c r="C207" s="8"/>
@@ -9957,7 +9954,7 @@
     </row>
     <row r="208" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A208" s="12" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="B208" s="14"/>
       <c r="C208" s="8"/>
@@ -9979,7 +9976,7 @@
     </row>
     <row r="209" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A209" s="12" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="B209" s="14"/>
       <c r="C209" s="8"/>
@@ -10001,7 +9998,7 @@
     </row>
     <row r="210" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A210" s="12" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B210" s="14"/>
       <c r="C210" s="8"/>
@@ -10023,7 +10020,7 @@
     </row>
     <row r="211" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A211" s="12" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="B211" s="14"/>
       <c r="C211" s="8"/>
@@ -10045,7 +10042,7 @@
     </row>
     <row r="212" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A212" s="12" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="B212" s="14"/>
       <c r="C212" s="8"/>
@@ -10067,7 +10064,7 @@
     </row>
     <row r="213" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A213" s="12" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="B213" s="14"/>
       <c r="C213" s="8"/>
@@ -10089,7 +10086,7 @@
     </row>
     <row r="214" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A214" s="12" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B214" s="14"/>
       <c r="C214" s="8"/>
@@ -10111,7 +10108,7 @@
     </row>
     <row r="215" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A215" s="12" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B215" s="14"/>
       <c r="C215" s="8"/>
@@ -10133,7 +10130,7 @@
     </row>
     <row r="216" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A216" s="12" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B216" s="14"/>
       <c r="C216" s="8"/>
@@ -10155,7 +10152,7 @@
     </row>
     <row r="217" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A217" s="12" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B217" s="14"/>
       <c r="C217" s="8"/>
@@ -10177,7 +10174,7 @@
     </row>
     <row r="218" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A218" s="12" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B218" s="14"/>
       <c r="C218" s="8"/>
@@ -10199,7 +10196,7 @@
     </row>
     <row r="219" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A219" s="12" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B219" s="14"/>
       <c r="C219" s="8"/>
@@ -10221,7 +10218,7 @@
     </row>
     <row r="220" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A220" s="12" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="B220" s="14"/>
       <c r="C220" s="8"/>
@@ -10243,7 +10240,7 @@
     </row>
     <row r="221" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A221" s="12" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="B221" s="14"/>
       <c r="C221" s="8"/>
@@ -10265,7 +10262,7 @@
     </row>
     <row r="222" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A222" s="12" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="B222" s="14"/>
       <c r="C222" s="8"/>
@@ -10287,7 +10284,7 @@
     </row>
     <row r="223" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A223" s="12" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="B223" s="14"/>
       <c r="C223" s="8"/>
@@ -10309,7 +10306,7 @@
     </row>
     <row r="224" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A224" s="12" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B224" s="14"/>
       <c r="C224" s="8"/>
@@ -10331,7 +10328,7 @@
     </row>
     <row r="225" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A225" s="12" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="B225" s="14"/>
       <c r="C225" s="8"/>
@@ -10353,7 +10350,7 @@
     </row>
     <row r="226" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A226" s="12" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="B226" s="14"/>
       <c r="C226" s="8"/>
@@ -10375,7 +10372,7 @@
     </row>
     <row r="227" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A227" s="12" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="B227" s="14"/>
       <c r="C227" s="8"/>
@@ -10397,7 +10394,7 @@
     </row>
     <row r="228" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A228" s="12" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="B228" s="14"/>
       <c r="C228" s="8"/>
@@ -10419,7 +10416,7 @@
     </row>
     <row r="229" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A229" s="12" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="B229" s="14"/>
       <c r="C229" s="8"/>
@@ -10441,7 +10438,7 @@
     </row>
     <row r="230" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A230" s="12" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="B230" s="14"/>
       <c r="C230" s="8"/>
@@ -10463,7 +10460,7 @@
     </row>
     <row r="231" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A231" s="12" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="B231" s="14"/>
       <c r="C231" s="8"/>
@@ -10485,7 +10482,7 @@
     </row>
     <row r="232" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A232" s="12" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="B232" s="14"/>
       <c r="C232" s="8"/>
@@ -10507,7 +10504,7 @@
     </row>
     <row r="233" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A233" s="12" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B233" s="14"/>
       <c r="C233" s="8"/>
@@ -10529,7 +10526,7 @@
     </row>
     <row r="234" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A234" s="12" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="B234" s="14"/>
       <c r="C234" s="8"/>
@@ -10551,7 +10548,7 @@
     </row>
     <row r="235" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A235" s="12" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="B235" s="14"/>
       <c r="C235" s="8"/>
@@ -10573,7 +10570,7 @@
     </row>
     <row r="236" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A236" s="12" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="B236" s="14"/>
       <c r="C236" s="8"/>
@@ -10595,7 +10592,7 @@
     </row>
     <row r="237" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A237" s="12" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="B237" s="14"/>
       <c r="C237" s="8"/>
@@ -10617,7 +10614,7 @@
     </row>
     <row r="238" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A238" s="12" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="B238" s="14"/>
       <c r="C238" s="8"/>
@@ -10639,7 +10636,7 @@
     </row>
     <row r="239" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A239" s="12" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="B239" s="14"/>
       <c r="C239" s="8"/>
@@ -10661,7 +10658,7 @@
     </row>
     <row r="240" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A240" s="12" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="B240" s="14"/>
       <c r="C240" s="8"/>
@@ -10683,7 +10680,7 @@
     </row>
     <row r="241" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A241" s="12" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="B241" s="14"/>
       <c r="C241" s="8"/>
@@ -10705,7 +10702,7 @@
     </row>
     <row r="242" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A242" s="12" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="B242" s="14"/>
       <c r="C242" s="8"/>
@@ -10727,7 +10724,7 @@
     </row>
     <row r="243" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A243" s="12" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="B243" s="14"/>
       <c r="C243" s="8"/>
@@ -10749,7 +10746,7 @@
     </row>
     <row r="244" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A244" s="12" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="B244" s="14"/>
       <c r="C244" s="8"/>
@@ -10771,7 +10768,7 @@
     </row>
     <row r="245" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A245" s="12" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B245" s="14"/>
       <c r="C245" s="8"/>
@@ -10793,7 +10790,7 @@
     </row>
     <row r="246" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A246" s="12" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="B246" s="14"/>
       <c r="C246" s="8"/>
@@ -10815,7 +10812,7 @@
     </row>
     <row r="247" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A247" s="12" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="B247" s="14"/>
       <c r="C247" s="8"/>
@@ -10837,7 +10834,7 @@
     </row>
     <row r="248" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A248" s="12" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="B248" s="14"/>
       <c r="C248" s="8"/>
@@ -10859,7 +10856,7 @@
     </row>
     <row r="249" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A249" s="12" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B249" s="14"/>
       <c r="C249" s="8"/>
@@ -10881,7 +10878,7 @@
     </row>
     <row r="250" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A250" s="12" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="B250" s="14"/>
       <c r="C250" s="8"/>
@@ -10903,7 +10900,7 @@
     </row>
     <row r="251" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A251" s="12" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="B251" s="14"/>
       <c r="C251" s="8"/>
@@ -10925,7 +10922,7 @@
     </row>
     <row r="252" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A252" s="12" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B252" s="14"/>
       <c r="C252" s="8"/>
@@ -10947,7 +10944,7 @@
     </row>
     <row r="253" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A253" s="12" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B253" s="14"/>
       <c r="C253" s="8"/>
@@ -10969,7 +10966,7 @@
     </row>
     <row r="254" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A254" s="12" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="B254" s="14"/>
       <c r="C254" s="8"/>
@@ -10991,7 +10988,7 @@
     </row>
     <row r="255" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A255" s="12" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B255" s="14"/>
       <c r="C255" s="8"/>
@@ -11013,7 +11010,7 @@
     </row>
     <row r="256" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A256" s="12" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="B256" s="14"/>
       <c r="C256" s="8"/>
@@ -11035,7 +11032,7 @@
     </row>
     <row r="257" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A257" s="12" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="B257" s="14"/>
       <c r="C257" s="8"/>
@@ -11120,7 +11117,7 @@
         <v>19</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="C2" s="22"/>
       <c r="D2" s="22"/>

</xml_diff>

<commit_message>
fix: correct CMP # implementation by incrementing at the last cycle
</commit_message>
<xml_diff>
--- a/docs/PandesalCPU Specs.xlsx
+++ b/docs/PandesalCPU Specs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shim Manaloto\Documents\PandesalCPU\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB83CD54-C28F-44B3-B16A-2F0686DE1791}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEDC3574-F98E-4777-BC98-DFEC00A5527B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{A2A5A835-37AC-4F29-881C-332D1F6F724B}"/>
   </bookViews>
@@ -2772,7 +2772,7 @@
   <dimension ref="A1:AJ257"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+      <selection activeCell="C2" sqref="C2:R74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5336,7 +5336,7 @@
         <v>292</v>
       </c>
       <c r="G45" s="9" t="s">
-        <v>332</v>
+        <v>346</v>
       </c>
       <c r="H45" s="10" t="s">
         <v>304</v>

</xml_diff>

<commit_message>
feat: implement LD0 abs, LD1 abs, LD2 abs, LD3 abs, and LD4 abs instructions
</commit_message>
<xml_diff>
--- a/docs/PandesalCPU Specs.xlsx
+++ b/docs/PandesalCPU Specs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shim Manaloto\Documents\PandesalCPU\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEDC3574-F98E-4777-BC98-DFEC00A5527B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{199EA3B8-0D48-4C7A-806F-E5EDD981D9E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{A2A5A835-37AC-4F29-881C-332D1F6F724B}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1683" uniqueCount="566">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1840" uniqueCount="583">
   <si>
     <t>000</t>
   </si>
@@ -1736,6 +1736,57 @@
   </si>
   <si>
     <t>1010 1111 000 0 0 00 0</t>
+  </si>
+  <si>
+    <t>ROM</t>
+  </si>
+  <si>
+    <t>0xC000 - 0xFFFF</t>
+  </si>
+  <si>
+    <t>LD0 #</t>
+  </si>
+  <si>
+    <t>LD1 #</t>
+  </si>
+  <si>
+    <t>LD2 #</t>
+  </si>
+  <si>
+    <t>LD3 #</t>
+  </si>
+  <si>
+    <t>LD4 #</t>
+  </si>
+  <si>
+    <t>1111 0011 000 0 0 01 1</t>
+  </si>
+  <si>
+    <t>1111 1011 000 0 0 01 1</t>
+  </si>
+  <si>
+    <t>1111 1100 000 0 0 01 1</t>
+  </si>
+  <si>
+    <t>1111 1101 000 0 0 01 1</t>
+  </si>
+  <si>
+    <t>1111 1110 000 0 0 01 1</t>
+  </si>
+  <si>
+    <t>LD0 abs</t>
+  </si>
+  <si>
+    <t>LD1 abs</t>
+  </si>
+  <si>
+    <t>LD2 abs</t>
+  </si>
+  <si>
+    <t>LD3 abs</t>
+  </si>
+  <si>
+    <t>LD4 abs</t>
   </si>
 </sst>
 </file>
@@ -2303,10 +2354,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E48F8AD-971A-4094-8D85-72B0AE25E8BF}">
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView zoomScale="114" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView topLeftCell="A3" zoomScale="114" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2338,7 +2389,7 @@
     <col min="35" max="35" width="10.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>256</v>
       </c>
@@ -2346,7 +2397,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -2374,8 +2425,11 @@
       <c r="K2" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L2" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2403,13 +2457,16 @@
       <c r="K3" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L3" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="F4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>57</v>
       </c>
@@ -2417,7 +2474,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>58</v>
       </c>
@@ -2425,8 +2482,8 @@
         <v>284</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="18.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" ht="18.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>59</v>
       </c>
@@ -2434,7 +2491,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>60</v>
       </c>
@@ -2451,7 +2508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>61</v>
       </c>
@@ -2468,7 +2525,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>62</v>
       </c>
@@ -2485,7 +2542,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>69</v>
       </c>
@@ -2502,7 +2559,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>64</v>
       </c>
@@ -2519,7 +2576,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -2536,7 +2593,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>63</v>
       </c>
@@ -2553,7 +2610,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>65</v>
       </c>
@@ -2771,8 +2828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC51F965-835D-4E82-9AC8-2752CA30592B}">
   <dimension ref="A1:AJ257"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:R74"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="73" zoomScaleNormal="25" workbookViewId="0">
+      <selection activeCell="B84" sqref="B80:B84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7000,7 +7057,9 @@
       <c r="A75" s="12" t="s">
         <v>249</v>
       </c>
-      <c r="B75" s="15"/>
+      <c r="B75" s="15" t="s">
+        <v>568</v>
+      </c>
       <c r="C75" s="9" t="s">
         <v>286</v>
       </c>
@@ -7010,25 +7069,53 @@
       <c r="E75" s="9" t="s">
         <v>288</v>
       </c>
-      <c r="F75" s="9"/>
-      <c r="G75" s="9"/>
-      <c r="H75" s="9"/>
-      <c r="I75" s="9"/>
-      <c r="J75" s="9"/>
-      <c r="K75" s="9"/>
-      <c r="L75" s="9"/>
-      <c r="M75" s="9"/>
-      <c r="N75" s="9"/>
-      <c r="O75" s="9"/>
-      <c r="P75" s="9"/>
-      <c r="Q75" s="9"/>
-      <c r="R75" s="8"/>
+      <c r="F75" s="9" t="s">
+        <v>573</v>
+      </c>
+      <c r="G75" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="H75" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="I75" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="J75" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="K75" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="L75" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="M75" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="N75" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="O75" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="P75" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q75" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="R75" s="10" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="76" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A76" s="12" t="s">
         <v>250</v>
       </c>
-      <c r="B76" s="15"/>
+      <c r="B76" s="15" t="s">
+        <v>569</v>
+      </c>
       <c r="C76" s="9" t="s">
         <v>286</v>
       </c>
@@ -7038,25 +7125,53 @@
       <c r="E76" s="9" t="s">
         <v>288</v>
       </c>
-      <c r="F76" s="9"/>
-      <c r="G76" s="9"/>
-      <c r="H76" s="9"/>
-      <c r="I76" s="9"/>
-      <c r="J76" s="9"/>
-      <c r="K76" s="9"/>
-      <c r="L76" s="9"/>
-      <c r="M76" s="9"/>
-      <c r="N76" s="9"/>
-      <c r="O76" s="9"/>
-      <c r="P76" s="9"/>
-      <c r="Q76" s="9"/>
-      <c r="R76" s="8"/>
+      <c r="F76" s="9" t="s">
+        <v>574</v>
+      </c>
+      <c r="G76" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="H76" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="I76" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="J76" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="K76" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="L76" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="M76" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="N76" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="O76" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="P76" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q76" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="R76" s="10" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="77" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A77" s="12" t="s">
         <v>251</v>
       </c>
-      <c r="B77" s="15"/>
+      <c r="B77" s="15" t="s">
+        <v>570</v>
+      </c>
       <c r="C77" s="9" t="s">
         <v>286</v>
       </c>
@@ -7066,25 +7181,53 @@
       <c r="E77" s="9" t="s">
         <v>288</v>
       </c>
-      <c r="F77" s="9"/>
-      <c r="G77" s="9"/>
-      <c r="H77" s="9"/>
-      <c r="I77" s="9"/>
-      <c r="J77" s="9"/>
-      <c r="K77" s="9"/>
-      <c r="L77" s="9"/>
-      <c r="M77" s="9"/>
-      <c r="N77" s="9"/>
-      <c r="O77" s="9"/>
-      <c r="P77" s="9"/>
-      <c r="Q77" s="9"/>
-      <c r="R77" s="8"/>
+      <c r="F77" s="9" t="s">
+        <v>575</v>
+      </c>
+      <c r="G77" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="H77" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="I77" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="J77" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="K77" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="L77" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="M77" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="N77" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="O77" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="P77" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q77" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="R77" s="10" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="78" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A78" s="12" t="s">
         <v>252</v>
       </c>
-      <c r="B78" s="15"/>
+      <c r="B78" s="15" t="s">
+        <v>571</v>
+      </c>
       <c r="C78" s="9" t="s">
         <v>286</v>
       </c>
@@ -7094,25 +7237,53 @@
       <c r="E78" s="9" t="s">
         <v>288</v>
       </c>
-      <c r="F78" s="9"/>
-      <c r="G78" s="9"/>
-      <c r="H78" s="9"/>
-      <c r="I78" s="9"/>
-      <c r="J78" s="9"/>
-      <c r="K78" s="9"/>
-      <c r="L78" s="9"/>
-      <c r="M78" s="9"/>
-      <c r="N78" s="9"/>
-      <c r="O78" s="9"/>
-      <c r="P78" s="9"/>
-      <c r="Q78" s="9"/>
-      <c r="R78" s="8"/>
+      <c r="F78" s="9" t="s">
+        <v>576</v>
+      </c>
+      <c r="G78" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="H78" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="I78" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="J78" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="K78" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="L78" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="M78" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="N78" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="O78" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="P78" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q78" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="R78" s="10" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="79" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A79" s="12" t="s">
         <v>253</v>
       </c>
-      <c r="B79" s="15"/>
+      <c r="B79" s="15" t="s">
+        <v>572</v>
+      </c>
       <c r="C79" s="9" t="s">
         <v>286</v>
       </c>
@@ -7122,129 +7293,325 @@
       <c r="E79" s="9" t="s">
         <v>288</v>
       </c>
-      <c r="F79" s="9"/>
-      <c r="G79" s="9"/>
-      <c r="H79" s="9"/>
-      <c r="I79" s="9"/>
-      <c r="J79" s="9"/>
-      <c r="K79" s="9"/>
-      <c r="L79" s="9"/>
-      <c r="M79" s="9"/>
-      <c r="N79" s="9"/>
-      <c r="O79" s="9"/>
-      <c r="P79" s="9"/>
-      <c r="Q79" s="9"/>
-      <c r="R79" s="8"/>
+      <c r="F79" s="9" t="s">
+        <v>577</v>
+      </c>
+      <c r="G79" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="H79" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="I79" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="J79" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="K79" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="L79" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="M79" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="N79" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="O79" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="P79" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q79" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="R79" s="10" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="80" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A80" s="12" t="s">
         <v>254</v>
       </c>
-      <c r="B80" s="15"/>
-      <c r="C80" s="9"/>
-      <c r="D80" s="9"/>
-      <c r="E80" s="9"/>
-      <c r="F80" s="9"/>
-      <c r="G80" s="9"/>
-      <c r="H80" s="9"/>
-      <c r="I80" s="9"/>
-      <c r="J80" s="9"/>
-      <c r="K80" s="9"/>
-      <c r="L80" s="9"/>
-      <c r="M80" s="9"/>
-      <c r="N80" s="9"/>
-      <c r="O80" s="9"/>
-      <c r="P80" s="9"/>
-      <c r="Q80" s="9"/>
-      <c r="R80" s="8"/>
+      <c r="B80" s="15" t="s">
+        <v>578</v>
+      </c>
+      <c r="C80" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="D80" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="E80" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="F80" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="G80" s="9" t="s">
+        <v>319</v>
+      </c>
+      <c r="H80" s="9" t="s">
+        <v>335</v>
+      </c>
+      <c r="I80" s="9" t="s">
+        <v>573</v>
+      </c>
+      <c r="J80" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="K80" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="L80" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="M80" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="N80" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="O80" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="P80" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q80" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="R80" s="10" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="81" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A81" s="12" t="s">
         <v>255</v>
       </c>
-      <c r="B81" s="15"/>
-      <c r="C81" s="9"/>
-      <c r="D81" s="9"/>
-      <c r="E81" s="9"/>
-      <c r="F81" s="9"/>
-      <c r="G81" s="9"/>
-      <c r="H81" s="9"/>
-      <c r="I81" s="9"/>
-      <c r="J81" s="9"/>
-      <c r="K81" s="9"/>
-      <c r="L81" s="9"/>
-      <c r="M81" s="9"/>
-      <c r="N81" s="9"/>
-      <c r="O81" s="9"/>
-      <c r="P81" s="9"/>
-      <c r="Q81" s="9"/>
-      <c r="R81" s="8"/>
+      <c r="B81" s="15" t="s">
+        <v>579</v>
+      </c>
+      <c r="C81" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="D81" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="E81" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="F81" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="G81" s="9" t="s">
+        <v>319</v>
+      </c>
+      <c r="H81" s="9" t="s">
+        <v>335</v>
+      </c>
+      <c r="I81" s="9" t="s">
+        <v>574</v>
+      </c>
+      <c r="J81" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="K81" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="L81" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="M81" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="N81" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="O81" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="P81" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q81" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="R81" s="10" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="82" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A82" s="12" t="s">
         <v>365</v>
       </c>
-      <c r="B82" s="15"/>
-      <c r="C82" s="9"/>
-      <c r="D82" s="9"/>
-      <c r="E82" s="9"/>
-      <c r="F82" s="9"/>
-      <c r="G82" s="9"/>
-      <c r="H82" s="9"/>
-      <c r="I82" s="9"/>
-      <c r="J82" s="9"/>
-      <c r="K82" s="9"/>
-      <c r="L82" s="9"/>
-      <c r="M82" s="9"/>
-      <c r="N82" s="9"/>
-      <c r="O82" s="9"/>
-      <c r="P82" s="9"/>
-      <c r="Q82" s="9"/>
-      <c r="R82" s="8"/>
+      <c r="B82" s="15" t="s">
+        <v>580</v>
+      </c>
+      <c r="C82" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="D82" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="E82" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="F82" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="G82" s="9" t="s">
+        <v>319</v>
+      </c>
+      <c r="H82" s="9" t="s">
+        <v>335</v>
+      </c>
+      <c r="I82" s="9" t="s">
+        <v>575</v>
+      </c>
+      <c r="J82" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="K82" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="L82" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="M82" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="N82" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="O82" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="P82" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q82" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="R82" s="10" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="83" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A83" s="12" t="s">
         <v>366</v>
       </c>
-      <c r="B83" s="15"/>
-      <c r="C83" s="9"/>
-      <c r="D83" s="9"/>
-      <c r="E83" s="9"/>
-      <c r="F83" s="9"/>
-      <c r="G83" s="9"/>
-      <c r="H83" s="9"/>
-      <c r="I83" s="9"/>
-      <c r="J83" s="9"/>
-      <c r="K83" s="9"/>
-      <c r="L83" s="9"/>
-      <c r="M83" s="9"/>
-      <c r="N83" s="9"/>
-      <c r="O83" s="9"/>
-      <c r="P83" s="9"/>
-      <c r="Q83" s="9"/>
-      <c r="R83" s="8"/>
+      <c r="B83" s="15" t="s">
+        <v>581</v>
+      </c>
+      <c r="C83" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="D83" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="E83" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="F83" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="G83" s="9" t="s">
+        <v>319</v>
+      </c>
+      <c r="H83" s="9" t="s">
+        <v>335</v>
+      </c>
+      <c r="I83" s="9" t="s">
+        <v>576</v>
+      </c>
+      <c r="J83" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="K83" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="L83" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="M83" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="N83" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="O83" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="P83" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q83" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="R83" s="10" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="84" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A84" s="12" t="s">
         <v>367</v>
       </c>
-      <c r="B84" s="15"/>
-      <c r="C84" s="9"/>
-      <c r="D84" s="9"/>
-      <c r="E84" s="9"/>
-      <c r="F84" s="9"/>
-      <c r="G84" s="9"/>
-      <c r="H84" s="9"/>
-      <c r="I84" s="9"/>
-      <c r="J84" s="9"/>
-      <c r="K84" s="9"/>
-      <c r="L84" s="9"/>
-      <c r="M84" s="9"/>
-      <c r="N84" s="9"/>
-      <c r="O84" s="9"/>
-      <c r="P84" s="9"/>
-      <c r="Q84" s="9"/>
-      <c r="R84" s="8"/>
+      <c r="B84" s="15" t="s">
+        <v>582</v>
+      </c>
+      <c r="C84" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="D84" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="E84" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="F84" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="G84" s="9" t="s">
+        <v>319</v>
+      </c>
+      <c r="H84" s="9" t="s">
+        <v>335</v>
+      </c>
+      <c r="I84" s="9" t="s">
+        <v>577</v>
+      </c>
+      <c r="J84" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="K84" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="L84" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="M84" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="N84" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="O84" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="P84" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q84" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="R84" s="10" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="85" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A85" s="12" t="s">

</xml_diff>

<commit_message>
feat: implement TA0 impl, TA1 impl, TA2 impl, TA3 impl, and TA4 instructions
</commit_message>
<xml_diff>
--- a/docs/PandesalCPU Specs.xlsx
+++ b/docs/PandesalCPU Specs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shim Manaloto\Documents\PandesalCPU\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{199EA3B8-0D48-4C7A-806F-E5EDD981D9E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A1B200-3B25-4039-9029-A464911F623F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{A2A5A835-37AC-4F29-881C-332D1F6F724B}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1840" uniqueCount="583">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1925" uniqueCount="593">
   <si>
     <t>000</t>
   </si>
@@ -1787,6 +1787,36 @@
   </si>
   <si>
     <t>LD4 abs</t>
+  </si>
+  <si>
+    <t>TA0 impl</t>
+  </si>
+  <si>
+    <t>TA1 impl</t>
+  </si>
+  <si>
+    <t>TA2 impl</t>
+  </si>
+  <si>
+    <t>TA3 impl</t>
+  </si>
+  <si>
+    <t>TA4 impl</t>
+  </si>
+  <si>
+    <t>0110 1100 000 0 0 01 0</t>
+  </si>
+  <si>
+    <t>0110 0011 000 0 0 01 0</t>
+  </si>
+  <si>
+    <t>0110 1011 000 0 0 01 0</t>
+  </si>
+  <si>
+    <t>0110 1101 000 0 0 01 0</t>
+  </si>
+  <si>
+    <t>0110 1110 000 0 0 01 0</t>
   </si>
 </sst>
 </file>
@@ -2828,8 +2858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC51F965-835D-4E82-9AC8-2752CA30592B}">
   <dimension ref="A1:AJ257"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="73" zoomScaleNormal="25" workbookViewId="0">
-      <selection activeCell="B84" sqref="B80:B84"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="98" zoomScaleNormal="25" workbookViewId="0">
+      <selection activeCell="B90" sqref="B90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7617,111 +7647,281 @@
       <c r="A85" s="12" t="s">
         <v>368</v>
       </c>
-      <c r="B85" s="15"/>
-      <c r="C85" s="9"/>
-      <c r="D85" s="9"/>
-      <c r="E85" s="9"/>
-      <c r="F85" s="9"/>
-      <c r="G85" s="9"/>
-      <c r="H85" s="9"/>
-      <c r="I85" s="9"/>
-      <c r="J85" s="9"/>
-      <c r="K85" s="9"/>
-      <c r="L85" s="9"/>
-      <c r="M85" s="9"/>
-      <c r="N85" s="9"/>
-      <c r="O85" s="9"/>
-      <c r="P85" s="9"/>
-      <c r="Q85" s="8"/>
-      <c r="R85" s="8"/>
+      <c r="B85" s="15" t="s">
+        <v>583</v>
+      </c>
+      <c r="C85" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="D85" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="E85" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="F85" s="9" t="s">
+        <v>589</v>
+      </c>
+      <c r="G85" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="H85" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="I85" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="J85" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="K85" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="L85" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="M85" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="N85" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="O85" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="P85" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q85" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="R85" s="10" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="86" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A86" s="12" t="s">
         <v>369</v>
       </c>
-      <c r="B86" s="15"/>
-      <c r="C86" s="9"/>
-      <c r="D86" s="9"/>
-      <c r="E86" s="9"/>
-      <c r="F86" s="9"/>
-      <c r="G86" s="9"/>
-      <c r="H86" s="9"/>
-      <c r="I86" s="9"/>
-      <c r="J86" s="9"/>
-      <c r="K86" s="9"/>
-      <c r="L86" s="9"/>
-      <c r="M86" s="9"/>
-      <c r="N86" s="9"/>
-      <c r="O86" s="9"/>
-      <c r="P86" s="9"/>
-      <c r="Q86" s="8"/>
-      <c r="R86" s="8"/>
+      <c r="B86" s="15" t="s">
+        <v>584</v>
+      </c>
+      <c r="C86" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="D86" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="E86" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="F86" s="9" t="s">
+        <v>590</v>
+      </c>
+      <c r="G86" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="H86" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="I86" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="J86" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="K86" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="L86" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="M86" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="N86" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="O86" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="P86" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q86" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="R86" s="10" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="87" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A87" s="12" t="s">
         <v>370</v>
       </c>
-      <c r="B87" s="14"/>
-      <c r="C87" s="8"/>
-      <c r="D87" s="8"/>
-      <c r="E87" s="8"/>
-      <c r="F87" s="8"/>
-      <c r="G87" s="8"/>
-      <c r="H87" s="8"/>
-      <c r="I87" s="8"/>
-      <c r="J87" s="8"/>
-      <c r="K87" s="8"/>
-      <c r="L87" s="8"/>
-      <c r="M87" s="8"/>
-      <c r="N87" s="8"/>
-      <c r="O87" s="8"/>
-      <c r="P87" s="8"/>
-      <c r="Q87" s="8"/>
-      <c r="R87" s="8"/>
+      <c r="B87" s="14" t="s">
+        <v>585</v>
+      </c>
+      <c r="C87" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="D87" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="E87" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="F87" s="9" t="s">
+        <v>588</v>
+      </c>
+      <c r="G87" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="H87" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="I87" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="J87" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="K87" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="L87" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="M87" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="N87" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="O87" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="P87" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q87" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="R87" s="10" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="88" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A88" s="12" t="s">
         <v>371</v>
       </c>
-      <c r="B88" s="14"/>
-      <c r="C88" s="8"/>
-      <c r="D88" s="8"/>
-      <c r="E88" s="8"/>
-      <c r="F88" s="8"/>
-      <c r="G88" s="8"/>
-      <c r="H88" s="8"/>
-      <c r="I88" s="8"/>
-      <c r="J88" s="8"/>
-      <c r="K88" s="8"/>
-      <c r="L88" s="8"/>
-      <c r="M88" s="8"/>
-      <c r="N88" s="8"/>
-      <c r="O88" s="8"/>
-      <c r="P88" s="8"/>
-      <c r="Q88" s="8"/>
-      <c r="R88" s="8"/>
+      <c r="B88" s="14" t="s">
+        <v>586</v>
+      </c>
+      <c r="C88" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="D88" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="E88" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="F88" s="9" t="s">
+        <v>591</v>
+      </c>
+      <c r="G88" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="H88" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="I88" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="J88" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="K88" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="L88" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="M88" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="N88" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="O88" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="P88" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q88" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="R88" s="10" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="89" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A89" s="12" t="s">
         <v>372</v>
       </c>
-      <c r="B89" s="14"/>
-      <c r="C89" s="8"/>
-      <c r="D89" s="8"/>
-      <c r="E89" s="8"/>
-      <c r="F89" s="8"/>
-      <c r="G89" s="8"/>
-      <c r="H89" s="8"/>
-      <c r="I89" s="8"/>
-      <c r="J89" s="8"/>
-      <c r="K89" s="8"/>
-      <c r="L89" s="8"/>
-      <c r="M89" s="8"/>
-      <c r="N89" s="8"/>
-      <c r="O89" s="8"/>
-      <c r="P89" s="8"/>
-      <c r="Q89" s="8"/>
-      <c r="R89" s="8"/>
+      <c r="B89" s="14" t="s">
+        <v>587</v>
+      </c>
+      <c r="C89" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="D89" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="E89" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="F89" s="9" t="s">
+        <v>592</v>
+      </c>
+      <c r="G89" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="H89" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="I89" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="J89" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="K89" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="L89" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="M89" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="N89" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="O89" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="P89" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q89" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="R89" s="10" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="90" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A90" s="12" t="s">

</xml_diff>

<commit_message>
feat: implement T0A impl, T1A impl, T2A impl, T3A impl, T4A impl instructions
</commit_message>
<xml_diff>
--- a/docs/PandesalCPU Specs.xlsx
+++ b/docs/PandesalCPU Specs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shim Manaloto\Documents\PandesalCPU\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A1B200-3B25-4039-9029-A464911F623F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{597A2704-5D5E-46D9-B6B7-254731C2E5D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{A2A5A835-37AC-4F29-881C-332D1F6F724B}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1925" uniqueCount="593">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2010" uniqueCount="603">
   <si>
     <t>000</t>
   </si>
@@ -1817,6 +1817,36 @@
   </si>
   <si>
     <t>0110 1110 000 0 0 01 0</t>
+  </si>
+  <si>
+    <t>T0A impl</t>
+  </si>
+  <si>
+    <t>T1A impl</t>
+  </si>
+  <si>
+    <t>T2A impl</t>
+  </si>
+  <si>
+    <t>T3A impl</t>
+  </si>
+  <si>
+    <t>T4A impl</t>
+  </si>
+  <si>
+    <t>0011 0110 000 0 0 01 0</t>
+  </si>
+  <si>
+    <t>1011 0110 000 0 0 01 0</t>
+  </si>
+  <si>
+    <t>1100 0110 000 0 0 01 0</t>
+  </si>
+  <si>
+    <t>1101 0110 000 0 0 01 0</t>
+  </si>
+  <si>
+    <t>1110 0110 000 0 0 01 0</t>
   </si>
 </sst>
 </file>
@@ -2858,8 +2888,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC51F965-835D-4E82-9AC8-2752CA30592B}">
   <dimension ref="A1:AJ257"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="98" zoomScaleNormal="25" workbookViewId="0">
-      <selection activeCell="B90" sqref="B90"/>
+    <sheetView tabSelected="1" topLeftCell="A86" zoomScale="98" zoomScaleNormal="25" workbookViewId="0">
+      <selection activeCell="B94" sqref="B90:B94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7927,111 +7957,281 @@
       <c r="A90" s="12" t="s">
         <v>373</v>
       </c>
-      <c r="B90" s="14"/>
-      <c r="C90" s="8"/>
-      <c r="D90" s="8"/>
-      <c r="E90" s="8"/>
-      <c r="F90" s="8"/>
-      <c r="G90" s="8"/>
-      <c r="H90" s="8"/>
-      <c r="I90" s="8"/>
-      <c r="J90" s="8"/>
-      <c r="K90" s="8"/>
-      <c r="L90" s="8"/>
-      <c r="M90" s="8"/>
-      <c r="N90" s="8"/>
-      <c r="O90" s="8"/>
-      <c r="P90" s="8"/>
-      <c r="Q90" s="8"/>
-      <c r="R90" s="8"/>
+      <c r="B90" s="14" t="s">
+        <v>593</v>
+      </c>
+      <c r="C90" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="D90" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="E90" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="F90" s="9" t="s">
+        <v>598</v>
+      </c>
+      <c r="G90" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="H90" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="I90" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="J90" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="K90" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="L90" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="M90" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="N90" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="O90" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="P90" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q90" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="R90" s="10" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="91" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A91" s="12" t="s">
         <v>374</v>
       </c>
-      <c r="B91" s="14"/>
-      <c r="C91" s="8"/>
-      <c r="D91" s="8"/>
-      <c r="E91" s="8"/>
-      <c r="F91" s="8"/>
-      <c r="G91" s="8"/>
-      <c r="H91" s="8"/>
-      <c r="I91" s="8"/>
-      <c r="J91" s="8"/>
-      <c r="K91" s="8"/>
-      <c r="L91" s="8"/>
-      <c r="M91" s="8"/>
-      <c r="N91" s="8"/>
-      <c r="O91" s="8"/>
-      <c r="P91" s="8"/>
-      <c r="Q91" s="8"/>
-      <c r="R91" s="8"/>
+      <c r="B91" s="14" t="s">
+        <v>594</v>
+      </c>
+      <c r="C91" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="D91" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="E91" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="F91" s="9" t="s">
+        <v>599</v>
+      </c>
+      <c r="G91" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="H91" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="I91" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="J91" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="K91" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="L91" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="M91" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="N91" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="O91" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="P91" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q91" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="R91" s="10" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="92" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A92" s="12" t="s">
         <v>375</v>
       </c>
-      <c r="B92" s="14"/>
-      <c r="C92" s="8"/>
-      <c r="D92" s="8"/>
-      <c r="E92" s="8"/>
-      <c r="F92" s="8"/>
-      <c r="G92" s="8"/>
-      <c r="H92" s="8"/>
-      <c r="I92" s="8"/>
-      <c r="J92" s="8"/>
-      <c r="K92" s="8"/>
-      <c r="L92" s="8"/>
-      <c r="M92" s="8"/>
-      <c r="N92" s="8"/>
-      <c r="O92" s="8"/>
-      <c r="P92" s="8"/>
-      <c r="Q92" s="8"/>
-      <c r="R92" s="8"/>
+      <c r="B92" s="14" t="s">
+        <v>595</v>
+      </c>
+      <c r="C92" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="D92" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="E92" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="F92" s="9" t="s">
+        <v>600</v>
+      </c>
+      <c r="G92" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="H92" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="I92" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="J92" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="K92" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="L92" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="M92" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="N92" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="O92" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="P92" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q92" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="R92" s="10" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="93" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A93" s="12" t="s">
         <v>376</v>
       </c>
-      <c r="B93" s="14"/>
-      <c r="C93" s="8"/>
-      <c r="D93" s="8"/>
-      <c r="E93" s="8"/>
-      <c r="F93" s="8"/>
-      <c r="G93" s="8"/>
-      <c r="H93" s="8"/>
-      <c r="I93" s="8"/>
-      <c r="J93" s="8"/>
-      <c r="K93" s="8"/>
-      <c r="L93" s="8"/>
-      <c r="M93" s="8"/>
-      <c r="N93" s="8"/>
-      <c r="O93" s="8"/>
-      <c r="P93" s="8"/>
-      <c r="Q93" s="8"/>
-      <c r="R93" s="8"/>
+      <c r="B93" s="14" t="s">
+        <v>596</v>
+      </c>
+      <c r="C93" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="D93" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="E93" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="F93" s="9" t="s">
+        <v>601</v>
+      </c>
+      <c r="G93" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="H93" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="I93" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="J93" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="K93" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="L93" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="M93" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="N93" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="O93" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="P93" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q93" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="R93" s="10" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="94" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A94" s="12" t="s">
         <v>377</v>
       </c>
-      <c r="B94" s="14"/>
-      <c r="C94" s="8"/>
-      <c r="D94" s="8"/>
-      <c r="E94" s="8"/>
-      <c r="F94" s="8"/>
-      <c r="G94" s="8"/>
-      <c r="H94" s="8"/>
-      <c r="I94" s="8"/>
-      <c r="J94" s="8"/>
-      <c r="K94" s="8"/>
-      <c r="L94" s="8"/>
-      <c r="M94" s="8"/>
-      <c r="N94" s="8"/>
-      <c r="O94" s="8"/>
-      <c r="P94" s="8"/>
-      <c r="Q94" s="8"/>
-      <c r="R94" s="8"/>
+      <c r="B94" s="14" t="s">
+        <v>597</v>
+      </c>
+      <c r="C94" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="D94" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="E94" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="F94" s="9" t="s">
+        <v>602</v>
+      </c>
+      <c r="G94" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="H94" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="I94" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="J94" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="K94" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="L94" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="M94" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="N94" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="O94" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="P94" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q94" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="R94" s="10" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="95" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A95" s="12" t="s">

</xml_diff>

<commit_message>
feat: implement TX0 impl, TX1 impl, TX2 impl, TX3 impl, and TX4 impl instructions
</commit_message>
<xml_diff>
--- a/docs/PandesalCPU Specs.xlsx
+++ b/docs/PandesalCPU Specs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shim Manaloto\Documents\PandesalCPU\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{597A2704-5D5E-46D9-B6B7-254731C2E5D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C818091-75FC-4635-BE80-044EB576EC1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{A2A5A835-37AC-4F29-881C-332D1F6F724B}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2010" uniqueCount="603">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2095" uniqueCount="613">
   <si>
     <t>000</t>
   </si>
@@ -1847,6 +1847,36 @@
   </si>
   <si>
     <t>1110 0110 000 0 0 01 0</t>
+  </si>
+  <si>
+    <t>TX0 impl</t>
+  </si>
+  <si>
+    <t>TX1 impl</t>
+  </si>
+  <si>
+    <t>TX2 impl</t>
+  </si>
+  <si>
+    <t>TX3 impl</t>
+  </si>
+  <si>
+    <t>TX4 impl</t>
+  </si>
+  <si>
+    <t>1001 0011 000 0 0 01 0</t>
+  </si>
+  <si>
+    <t>1001 1011 000 0 0 01 0</t>
+  </si>
+  <si>
+    <t>1001 1100 000 0 0 01 0</t>
+  </si>
+  <si>
+    <t>1001 1101 000 0 0 01 0</t>
+  </si>
+  <si>
+    <t>1001 1110 000 0 0 01 0</t>
   </si>
 </sst>
 </file>
@@ -2888,8 +2918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC51F965-835D-4E82-9AC8-2752CA30592B}">
   <dimension ref="A1:AJ257"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" zoomScale="98" zoomScaleNormal="25" workbookViewId="0">
-      <selection activeCell="B94" sqref="B90:B94"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="98" zoomScaleNormal="25" workbookViewId="0">
+      <selection activeCell="B99" sqref="B95:B99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8237,111 +8267,281 @@
       <c r="A95" s="12" t="s">
         <v>378</v>
       </c>
-      <c r="B95" s="14"/>
-      <c r="C95" s="8"/>
-      <c r="D95" s="8"/>
-      <c r="E95" s="8"/>
-      <c r="F95" s="8"/>
-      <c r="G95" s="8"/>
-      <c r="H95" s="8"/>
-      <c r="I95" s="8"/>
-      <c r="J95" s="8"/>
-      <c r="K95" s="8"/>
-      <c r="L95" s="8"/>
-      <c r="M95" s="8"/>
-      <c r="N95" s="8"/>
-      <c r="O95" s="8"/>
-      <c r="P95" s="8"/>
-      <c r="Q95" s="8"/>
-      <c r="R95" s="8"/>
+      <c r="B95" s="14" t="s">
+        <v>603</v>
+      </c>
+      <c r="C95" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="D95" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="E95" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="F95" s="9" t="s">
+        <v>608</v>
+      </c>
+      <c r="G95" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="H95" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="I95" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="J95" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="K95" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="L95" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="M95" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="N95" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="O95" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="P95" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q95" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="R95" s="10" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="96" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A96" s="12" t="s">
         <v>379</v>
       </c>
-      <c r="B96" s="14"/>
-      <c r="C96" s="8"/>
-      <c r="D96" s="8"/>
-      <c r="E96" s="8"/>
-      <c r="F96" s="8"/>
-      <c r="G96" s="8"/>
-      <c r="H96" s="8"/>
-      <c r="I96" s="8"/>
-      <c r="J96" s="8"/>
-      <c r="K96" s="8"/>
-      <c r="L96" s="8"/>
-      <c r="M96" s="8"/>
-      <c r="N96" s="8"/>
-      <c r="O96" s="8"/>
-      <c r="P96" s="8"/>
-      <c r="Q96" s="8"/>
-      <c r="R96" s="8"/>
+      <c r="B96" s="14" t="s">
+        <v>604</v>
+      </c>
+      <c r="C96" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="D96" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="E96" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="F96" s="9" t="s">
+        <v>609</v>
+      </c>
+      <c r="G96" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="H96" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="I96" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="J96" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="K96" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="L96" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="M96" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="N96" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="O96" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="P96" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q96" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="R96" s="10" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="97" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A97" s="12" t="s">
         <v>380</v>
       </c>
-      <c r="B97" s="14"/>
-      <c r="C97" s="8"/>
-      <c r="D97" s="8"/>
-      <c r="E97" s="8"/>
-      <c r="F97" s="8"/>
-      <c r="G97" s="8"/>
-      <c r="H97" s="8"/>
-      <c r="I97" s="8"/>
-      <c r="J97" s="8"/>
-      <c r="K97" s="8"/>
-      <c r="L97" s="8"/>
-      <c r="M97" s="8"/>
-      <c r="N97" s="8"/>
-      <c r="O97" s="8"/>
-      <c r="P97" s="8"/>
-      <c r="Q97" s="8"/>
-      <c r="R97" s="8"/>
+      <c r="B97" s="14" t="s">
+        <v>605</v>
+      </c>
+      <c r="C97" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="D97" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="E97" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="F97" s="9" t="s">
+        <v>610</v>
+      </c>
+      <c r="G97" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="H97" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="I97" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="J97" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="K97" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="L97" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="M97" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="N97" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="O97" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="P97" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q97" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="R97" s="10" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="98" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A98" s="12" t="s">
         <v>381</v>
       </c>
-      <c r="B98" s="14"/>
-      <c r="C98" s="8"/>
-      <c r="D98" s="8"/>
-      <c r="E98" s="8"/>
-      <c r="F98" s="8"/>
-      <c r="G98" s="8"/>
-      <c r="H98" s="8"/>
-      <c r="I98" s="8"/>
-      <c r="J98" s="8"/>
-      <c r="K98" s="8"/>
-      <c r="L98" s="8"/>
-      <c r="M98" s="8"/>
-      <c r="N98" s="8"/>
-      <c r="O98" s="8"/>
-      <c r="P98" s="8"/>
-      <c r="Q98" s="8"/>
-      <c r="R98" s="8"/>
+      <c r="B98" s="14" t="s">
+        <v>606</v>
+      </c>
+      <c r="C98" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="D98" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="E98" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="F98" s="9" t="s">
+        <v>611</v>
+      </c>
+      <c r="G98" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="H98" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="I98" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="J98" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="K98" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="L98" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="M98" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="N98" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="O98" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="P98" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q98" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="R98" s="10" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="99" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A99" s="12" t="s">
         <v>382</v>
       </c>
-      <c r="B99" s="14"/>
-      <c r="C99" s="8"/>
-      <c r="D99" s="8"/>
-      <c r="E99" s="8"/>
-      <c r="F99" s="8"/>
-      <c r="G99" s="8"/>
-      <c r="H99" s="8"/>
-      <c r="I99" s="8"/>
-      <c r="J99" s="8"/>
-      <c r="K99" s="8"/>
-      <c r="L99" s="8"/>
-      <c r="M99" s="8"/>
-      <c r="N99" s="8"/>
-      <c r="O99" s="8"/>
-      <c r="P99" s="8"/>
-      <c r="Q99" s="8"/>
-      <c r="R99" s="8"/>
+      <c r="B99" s="14" t="s">
+        <v>607</v>
+      </c>
+      <c r="C99" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="D99" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="E99" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="F99" s="9" t="s">
+        <v>612</v>
+      </c>
+      <c r="G99" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="H99" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="I99" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="J99" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="K99" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="L99" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="M99" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="N99" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="O99" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="P99" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q99" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="R99" s="10" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="100" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A100" s="12" t="s">

</xml_diff>

<commit_message>
feat: implement T0X impl, T1X impl, T2X impl, T3X impl, and T4X impl instructions
</commit_message>
<xml_diff>
--- a/docs/PandesalCPU Specs.xlsx
+++ b/docs/PandesalCPU Specs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shim Manaloto\Documents\PandesalCPU\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C818091-75FC-4635-BE80-044EB576EC1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68DD5BC1-6FF5-4931-9D59-45E4E833EF3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{A2A5A835-37AC-4F29-881C-332D1F6F724B}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2095" uniqueCount="613">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2180" uniqueCount="623">
   <si>
     <t>000</t>
   </si>
@@ -1877,6 +1877,36 @@
   </si>
   <si>
     <t>1001 1110 000 0 0 01 0</t>
+  </si>
+  <si>
+    <t>T0X impl</t>
+  </si>
+  <si>
+    <t>T1X impl</t>
+  </si>
+  <si>
+    <t>T2X impl</t>
+  </si>
+  <si>
+    <t>T3X impl</t>
+  </si>
+  <si>
+    <t>T4X impl</t>
+  </si>
+  <si>
+    <t>0011 1001 000 0 0 01 0</t>
+  </si>
+  <si>
+    <t>1011 1001 000 0 0 01 0</t>
+  </si>
+  <si>
+    <t>1100 1001 000 0 0 01 0</t>
+  </si>
+  <si>
+    <t>1101 1001 000 0 0 01 0</t>
+  </si>
+  <si>
+    <t>1110 1001 000 0 0 01 0</t>
   </si>
 </sst>
 </file>
@@ -2919,7 +2949,7 @@
   <dimension ref="A1:AJ257"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A85" zoomScale="98" zoomScaleNormal="25" workbookViewId="0">
-      <selection activeCell="B99" sqref="B95:B99"/>
+      <selection activeCell="G100" sqref="G100:R104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8547,111 +8577,281 @@
       <c r="A100" s="12" t="s">
         <v>383</v>
       </c>
-      <c r="B100" s="14"/>
-      <c r="C100" s="8"/>
-      <c r="D100" s="8"/>
-      <c r="E100" s="8"/>
-      <c r="F100" s="8"/>
-      <c r="G100" s="8"/>
-      <c r="H100" s="8"/>
-      <c r="I100" s="8"/>
-      <c r="J100" s="8"/>
-      <c r="K100" s="8"/>
-      <c r="L100" s="8"/>
-      <c r="M100" s="8"/>
-      <c r="N100" s="8"/>
-      <c r="O100" s="8"/>
-      <c r="P100" s="8"/>
-      <c r="Q100" s="8"/>
-      <c r="R100" s="8"/>
+      <c r="B100" s="14" t="s">
+        <v>613</v>
+      </c>
+      <c r="C100" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="D100" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="E100" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="F100" s="9" t="s">
+        <v>618</v>
+      </c>
+      <c r="G100" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="H100" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="I100" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="J100" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="K100" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="L100" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="M100" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="N100" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="O100" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="P100" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q100" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="R100" s="10" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="101" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A101" s="12" t="s">
         <v>384</v>
       </c>
-      <c r="B101" s="14"/>
-      <c r="C101" s="8"/>
-      <c r="D101" s="8"/>
-      <c r="E101" s="8"/>
-      <c r="F101" s="8"/>
-      <c r="G101" s="8"/>
-      <c r="H101" s="8"/>
-      <c r="I101" s="8"/>
-      <c r="J101" s="8"/>
-      <c r="K101" s="8"/>
-      <c r="L101" s="8"/>
-      <c r="M101" s="8"/>
-      <c r="N101" s="8"/>
-      <c r="O101" s="8"/>
-      <c r="P101" s="8"/>
-      <c r="Q101" s="8"/>
-      <c r="R101" s="8"/>
+      <c r="B101" s="14" t="s">
+        <v>614</v>
+      </c>
+      <c r="C101" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="D101" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="E101" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="F101" s="9" t="s">
+        <v>619</v>
+      </c>
+      <c r="G101" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="H101" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="I101" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="J101" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="K101" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="L101" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="M101" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="N101" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="O101" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="P101" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q101" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="R101" s="10" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="102" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A102" s="12" t="s">
         <v>385</v>
       </c>
-      <c r="B102" s="14"/>
-      <c r="C102" s="8"/>
-      <c r="D102" s="8"/>
-      <c r="E102" s="8"/>
-      <c r="F102" s="8"/>
-      <c r="G102" s="8"/>
-      <c r="H102" s="8"/>
-      <c r="I102" s="8"/>
-      <c r="J102" s="8"/>
-      <c r="K102" s="8"/>
-      <c r="L102" s="8"/>
-      <c r="M102" s="8"/>
-      <c r="N102" s="8"/>
-      <c r="O102" s="8"/>
-      <c r="P102" s="8"/>
-      <c r="Q102" s="8"/>
-      <c r="R102" s="8"/>
+      <c r="B102" s="14" t="s">
+        <v>615</v>
+      </c>
+      <c r="C102" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="D102" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="E102" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="F102" s="9" t="s">
+        <v>620</v>
+      </c>
+      <c r="G102" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="H102" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="I102" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="J102" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="K102" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="L102" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="M102" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="N102" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="O102" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="P102" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q102" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="R102" s="10" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="103" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A103" s="12" t="s">
         <v>386</v>
       </c>
-      <c r="B103" s="14"/>
-      <c r="C103" s="8"/>
-      <c r="D103" s="8"/>
-      <c r="E103" s="8"/>
-      <c r="F103" s="8"/>
-      <c r="G103" s="8"/>
-      <c r="H103" s="8"/>
-      <c r="I103" s="8"/>
-      <c r="J103" s="8"/>
-      <c r="K103" s="8"/>
-      <c r="L103" s="8"/>
-      <c r="M103" s="8"/>
-      <c r="N103" s="8"/>
-      <c r="O103" s="8"/>
-      <c r="P103" s="8"/>
-      <c r="Q103" s="8"/>
-      <c r="R103" s="8"/>
+      <c r="B103" s="14" t="s">
+        <v>616</v>
+      </c>
+      <c r="C103" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="D103" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="E103" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="F103" s="9" t="s">
+        <v>621</v>
+      </c>
+      <c r="G103" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="H103" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="I103" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="J103" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="K103" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="L103" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="M103" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="N103" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="O103" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="P103" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q103" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="R103" s="10" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="104" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A104" s="12" t="s">
         <v>387</v>
       </c>
-      <c r="B104" s="14"/>
-      <c r="C104" s="8"/>
-      <c r="D104" s="8"/>
-      <c r="E104" s="8"/>
-      <c r="F104" s="8"/>
-      <c r="G104" s="8"/>
-      <c r="H104" s="8"/>
-      <c r="I104" s="8"/>
-      <c r="J104" s="8"/>
-      <c r="K104" s="8"/>
-      <c r="L104" s="8"/>
-      <c r="M104" s="8"/>
-      <c r="N104" s="8"/>
-      <c r="O104" s="8"/>
-      <c r="P104" s="8"/>
-      <c r="Q104" s="8"/>
-      <c r="R104" s="8"/>
+      <c r="B104" s="14" t="s">
+        <v>617</v>
+      </c>
+      <c r="C104" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="D104" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="E104" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="F104" s="9" t="s">
+        <v>622</v>
+      </c>
+      <c r="G104" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="H104" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="I104" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="J104" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="K104" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="L104" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="M104" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="N104" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="O104" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="P104" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q104" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="R104" s="10" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="105" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A105" s="12" t="s">

</xml_diff>

<commit_message>
feat: implement TY0 impl, TY1 impl, TY2 impl, TY3 impl, and TY4 impl instructions
</commit_message>
<xml_diff>
--- a/docs/PandesalCPU Specs.xlsx
+++ b/docs/PandesalCPU Specs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shim Manaloto\Documents\PandesalCPU\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68DD5BC1-6FF5-4931-9D59-45E4E833EF3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97175CD3-2194-4E00-A28A-7705EAA15E1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{A2A5A835-37AC-4F29-881C-332D1F6F724B}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2180" uniqueCount="623">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2265" uniqueCount="633">
   <si>
     <t>000</t>
   </si>
@@ -1907,6 +1907,36 @@
   </si>
   <si>
     <t>1110 1001 000 0 0 01 0</t>
+  </si>
+  <si>
+    <t>TY0 impl</t>
+  </si>
+  <si>
+    <t>TY1 impl</t>
+  </si>
+  <si>
+    <t>TY2 impl</t>
+  </si>
+  <si>
+    <t>TY3 impl</t>
+  </si>
+  <si>
+    <t>TY4 impl</t>
+  </si>
+  <si>
+    <t>1010 0011 000 0 0 01 0</t>
+  </si>
+  <si>
+    <t>1010 1011 000 0 0 01 0</t>
+  </si>
+  <si>
+    <t>1010 1100 000 0 0 01 0</t>
+  </si>
+  <si>
+    <t>1010 1101 000 0 0 01 0</t>
+  </si>
+  <si>
+    <t>1010 1110 000 0 0 01 0</t>
   </si>
 </sst>
 </file>
@@ -2948,8 +2978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC51F965-835D-4E82-9AC8-2752CA30592B}">
   <dimension ref="A1:AJ257"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="98" zoomScaleNormal="25" workbookViewId="0">
-      <selection activeCell="G100" sqref="G100:R104"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="98" zoomScaleNormal="25" workbookViewId="0">
+      <selection activeCell="B109" sqref="B105:B109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8857,111 +8887,281 @@
       <c r="A105" s="12" t="s">
         <v>388</v>
       </c>
-      <c r="B105" s="14"/>
-      <c r="C105" s="8"/>
-      <c r="D105" s="8"/>
-      <c r="E105" s="8"/>
-      <c r="F105" s="8"/>
-      <c r="G105" s="8"/>
-      <c r="H105" s="8"/>
-      <c r="I105" s="8"/>
-      <c r="J105" s="8"/>
-      <c r="K105" s="8"/>
-      <c r="L105" s="8"/>
-      <c r="M105" s="8"/>
-      <c r="N105" s="8"/>
-      <c r="O105" s="8"/>
-      <c r="P105" s="8"/>
-      <c r="Q105" s="8"/>
-      <c r="R105" s="8"/>
+      <c r="B105" s="14" t="s">
+        <v>623</v>
+      </c>
+      <c r="C105" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="D105" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="E105" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="F105" s="9" t="s">
+        <v>628</v>
+      </c>
+      <c r="G105" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="H105" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="I105" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="J105" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="K105" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="L105" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="M105" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="N105" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="O105" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="P105" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q105" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="R105" s="10" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="106" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A106" s="12" t="s">
         <v>389</v>
       </c>
-      <c r="B106" s="14"/>
-      <c r="C106" s="8"/>
-      <c r="D106" s="8"/>
-      <c r="E106" s="8"/>
-      <c r="F106" s="8"/>
-      <c r="G106" s="8"/>
-      <c r="H106" s="8"/>
-      <c r="I106" s="8"/>
-      <c r="J106" s="8"/>
-      <c r="K106" s="8"/>
-      <c r="L106" s="8"/>
-      <c r="M106" s="8"/>
-      <c r="N106" s="8"/>
-      <c r="O106" s="8"/>
-      <c r="P106" s="8"/>
-      <c r="Q106" s="8"/>
-      <c r="R106" s="8"/>
+      <c r="B106" s="14" t="s">
+        <v>624</v>
+      </c>
+      <c r="C106" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="D106" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="E106" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="F106" s="9" t="s">
+        <v>629</v>
+      </c>
+      <c r="G106" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="H106" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="I106" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="J106" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="K106" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="L106" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="M106" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="N106" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="O106" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="P106" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q106" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="R106" s="10" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="107" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A107" s="12" t="s">
         <v>390</v>
       </c>
-      <c r="B107" s="14"/>
-      <c r="C107" s="8"/>
-      <c r="D107" s="8"/>
-      <c r="E107" s="8"/>
-      <c r="F107" s="8"/>
-      <c r="G107" s="8"/>
-      <c r="H107" s="8"/>
-      <c r="I107" s="8"/>
-      <c r="J107" s="8"/>
-      <c r="K107" s="8"/>
-      <c r="L107" s="8"/>
-      <c r="M107" s="8"/>
-      <c r="N107" s="8"/>
-      <c r="O107" s="8"/>
-      <c r="P107" s="8"/>
-      <c r="Q107" s="8"/>
-      <c r="R107" s="8"/>
+      <c r="B107" s="14" t="s">
+        <v>625</v>
+      </c>
+      <c r="C107" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="D107" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="E107" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="F107" s="9" t="s">
+        <v>630</v>
+      </c>
+      <c r="G107" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="H107" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="I107" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="J107" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="K107" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="L107" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="M107" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="N107" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="O107" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="P107" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q107" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="R107" s="10" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="108" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A108" s="12" t="s">
         <v>391</v>
       </c>
-      <c r="B108" s="14"/>
-      <c r="C108" s="8"/>
-      <c r="D108" s="8"/>
-      <c r="E108" s="8"/>
-      <c r="F108" s="8"/>
-      <c r="G108" s="8"/>
-      <c r="H108" s="8"/>
-      <c r="I108" s="8"/>
-      <c r="J108" s="8"/>
-      <c r="K108" s="8"/>
-      <c r="L108" s="8"/>
-      <c r="M108" s="8"/>
-      <c r="N108" s="8"/>
-      <c r="O108" s="8"/>
-      <c r="P108" s="8"/>
-      <c r="Q108" s="8"/>
-      <c r="R108" s="8"/>
+      <c r="B108" s="14" t="s">
+        <v>626</v>
+      </c>
+      <c r="C108" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="D108" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="E108" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="F108" s="9" t="s">
+        <v>631</v>
+      </c>
+      <c r="G108" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="H108" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="I108" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="J108" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="K108" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="L108" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="M108" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="N108" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="O108" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="P108" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q108" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="R108" s="10" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="109" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A109" s="12" t="s">
         <v>392</v>
       </c>
-      <c r="B109" s="14"/>
-      <c r="C109" s="8"/>
-      <c r="D109" s="8"/>
-      <c r="E109" s="8"/>
-      <c r="F109" s="8"/>
-      <c r="G109" s="8"/>
-      <c r="H109" s="8"/>
-      <c r="I109" s="8"/>
-      <c r="J109" s="8"/>
-      <c r="K109" s="8"/>
-      <c r="L109" s="8"/>
-      <c r="M109" s="8"/>
-      <c r="N109" s="8"/>
-      <c r="O109" s="8"/>
-      <c r="P109" s="8"/>
-      <c r="Q109" s="8"/>
-      <c r="R109" s="8"/>
+      <c r="B109" s="14" t="s">
+        <v>627</v>
+      </c>
+      <c r="C109" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="D109" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="E109" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="F109" s="9" t="s">
+        <v>632</v>
+      </c>
+      <c r="G109" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="H109" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="I109" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="J109" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="K109" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="L109" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="M109" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="N109" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="O109" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="P109" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q109" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="R109" s="10" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="110" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A110" s="12" t="s">

</xml_diff>

<commit_message>
feat: implement T0Y impl, T1Y impl, T2Y impl, T3Y impl, and T4Y impl instructions
</commit_message>
<xml_diff>
--- a/docs/PandesalCPU Specs.xlsx
+++ b/docs/PandesalCPU Specs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shim Manaloto\Documents\PandesalCPU\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97175CD3-2194-4E00-A28A-7705EAA15E1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF6CAF7C-439E-4A2E-8BDB-C561C35E95E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{A2A5A835-37AC-4F29-881C-332D1F6F724B}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2265" uniqueCount="633">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2350" uniqueCount="643">
   <si>
     <t>000</t>
   </si>
@@ -1937,6 +1937,36 @@
   </si>
   <si>
     <t>1010 1110 000 0 0 01 0</t>
+  </si>
+  <si>
+    <t>T0Y impl</t>
+  </si>
+  <si>
+    <t>T1Y impl</t>
+  </si>
+  <si>
+    <t>T2Y impl</t>
+  </si>
+  <si>
+    <t>T3Y impl</t>
+  </si>
+  <si>
+    <t>T4Y impl</t>
+  </si>
+  <si>
+    <t>0011 1010 000 0 0 01 0</t>
+  </si>
+  <si>
+    <t>1011 1010 000 0 0 01 0</t>
+  </si>
+  <si>
+    <t>1100 1010 000 0 0 01 0</t>
+  </si>
+  <si>
+    <t>1101 1010 000 0 0 01 0</t>
+  </si>
+  <si>
+    <t>1110 1010 000 0 0 01 0</t>
   </si>
 </sst>
 </file>
@@ -2978,8 +3008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC51F965-835D-4E82-9AC8-2752CA30592B}">
   <dimension ref="A1:AJ257"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="98" zoomScaleNormal="25" workbookViewId="0">
-      <selection activeCell="B109" sqref="B105:B109"/>
+    <sheetView tabSelected="1" topLeftCell="C103" zoomScale="98" zoomScaleNormal="25" workbookViewId="0">
+      <selection activeCell="G110" sqref="G110:R114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9167,111 +9197,281 @@
       <c r="A110" s="12" t="s">
         <v>393</v>
       </c>
-      <c r="B110" s="14"/>
-      <c r="C110" s="8"/>
-      <c r="D110" s="8"/>
-      <c r="E110" s="8"/>
-      <c r="F110" s="8"/>
-      <c r="G110" s="8"/>
-      <c r="H110" s="8"/>
-      <c r="I110" s="8"/>
-      <c r="J110" s="8"/>
-      <c r="K110" s="8"/>
-      <c r="L110" s="8"/>
-      <c r="M110" s="8"/>
-      <c r="N110" s="8"/>
-      <c r="O110" s="8"/>
-      <c r="P110" s="8"/>
-      <c r="Q110" s="8"/>
-      <c r="R110" s="8"/>
+      <c r="B110" s="14" t="s">
+        <v>633</v>
+      </c>
+      <c r="C110" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="D110" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="E110" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="F110" s="9" t="s">
+        <v>638</v>
+      </c>
+      <c r="G110" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="H110" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="I110" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="J110" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="K110" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="L110" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="M110" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="N110" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="O110" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="P110" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q110" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="R110" s="10" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="111" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A111" s="12" t="s">
         <v>394</v>
       </c>
-      <c r="B111" s="14"/>
-      <c r="C111" s="8"/>
-      <c r="D111" s="8"/>
-      <c r="E111" s="8"/>
-      <c r="F111" s="8"/>
-      <c r="G111" s="8"/>
-      <c r="H111" s="8"/>
-      <c r="I111" s="8"/>
-      <c r="J111" s="8"/>
-      <c r="K111" s="8"/>
-      <c r="L111" s="8"/>
-      <c r="M111" s="8"/>
-      <c r="N111" s="8"/>
-      <c r="O111" s="8"/>
-      <c r="P111" s="8"/>
-      <c r="Q111" s="8"/>
-      <c r="R111" s="8"/>
+      <c r="B111" s="14" t="s">
+        <v>634</v>
+      </c>
+      <c r="C111" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="D111" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="E111" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="F111" s="9" t="s">
+        <v>639</v>
+      </c>
+      <c r="G111" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="H111" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="I111" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="J111" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="K111" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="L111" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="M111" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="N111" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="O111" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="P111" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q111" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="R111" s="10" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="112" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A112" s="12" t="s">
         <v>395</v>
       </c>
-      <c r="B112" s="14"/>
-      <c r="C112" s="8"/>
-      <c r="D112" s="8"/>
-      <c r="E112" s="8"/>
-      <c r="F112" s="8"/>
-      <c r="G112" s="8"/>
-      <c r="H112" s="8"/>
-      <c r="I112" s="8"/>
-      <c r="J112" s="8"/>
-      <c r="K112" s="8"/>
-      <c r="L112" s="8"/>
-      <c r="M112" s="8"/>
-      <c r="N112" s="8"/>
-      <c r="O112" s="8"/>
-      <c r="P112" s="8"/>
-      <c r="Q112" s="8"/>
-      <c r="R112" s="8"/>
+      <c r="B112" s="14" t="s">
+        <v>635</v>
+      </c>
+      <c r="C112" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="D112" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="E112" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="F112" s="9" t="s">
+        <v>640</v>
+      </c>
+      <c r="G112" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="H112" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="I112" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="J112" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="K112" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="L112" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="M112" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="N112" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="O112" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="P112" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q112" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="R112" s="10" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="113" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A113" s="12" t="s">
         <v>396</v>
       </c>
-      <c r="B113" s="14"/>
-      <c r="C113" s="8"/>
-      <c r="D113" s="8"/>
-      <c r="E113" s="8"/>
-      <c r="F113" s="8"/>
-      <c r="G113" s="8"/>
-      <c r="H113" s="8"/>
-      <c r="I113" s="8"/>
-      <c r="J113" s="8"/>
-      <c r="K113" s="8"/>
-      <c r="L113" s="8"/>
-      <c r="M113" s="8"/>
-      <c r="N113" s="8"/>
-      <c r="O113" s="8"/>
-      <c r="P113" s="8"/>
-      <c r="Q113" s="8"/>
-      <c r="R113" s="8"/>
+      <c r="B113" s="14" t="s">
+        <v>636</v>
+      </c>
+      <c r="C113" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="D113" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="E113" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="F113" s="9" t="s">
+        <v>641</v>
+      </c>
+      <c r="G113" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="H113" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="I113" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="J113" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="K113" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="L113" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="M113" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="N113" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="O113" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="P113" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q113" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="R113" s="10" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="114" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A114" s="12" t="s">
         <v>397</v>
       </c>
-      <c r="B114" s="14"/>
-      <c r="C114" s="8"/>
-      <c r="D114" s="8"/>
-      <c r="E114" s="8"/>
-      <c r="F114" s="8"/>
-      <c r="G114" s="8"/>
-      <c r="H114" s="8"/>
-      <c r="I114" s="8"/>
-      <c r="J114" s="8"/>
-      <c r="K114" s="8"/>
-      <c r="L114" s="8"/>
-      <c r="M114" s="8"/>
-      <c r="N114" s="8"/>
-      <c r="O114" s="8"/>
-      <c r="P114" s="8"/>
-      <c r="Q114" s="8"/>
-      <c r="R114" s="8"/>
+      <c r="B114" s="14" t="s">
+        <v>637</v>
+      </c>
+      <c r="C114" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="D114" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="E114" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="F114" s="9" t="s">
+        <v>642</v>
+      </c>
+      <c r="G114" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="H114" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="I114" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="J114" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="K114" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="L114" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="M114" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="N114" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="O114" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="P114" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q114" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="R114" s="10" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="115" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A115" s="12" t="s">

</xml_diff>

<commit_message>
feat: implemented LDA ind instruction
</commit_message>
<xml_diff>
--- a/docs/PandesalCPU Specs.xlsx
+++ b/docs/PandesalCPU Specs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shim Manaloto\Documents\PandesalCPU\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF6CAF7C-439E-4A2E-8BDB-C561C35E95E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B18FF9A6-E593-4588-938E-5A0AC80718F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{A2A5A835-37AC-4F29-881C-332D1F6F724B}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2350" uniqueCount="643">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2367" uniqueCount="644">
   <si>
     <t>000</t>
   </si>
@@ -1967,6 +1967,9 @@
   </si>
   <si>
     <t>1110 1010 000 0 0 01 0</t>
+  </si>
+  <si>
+    <t>LDA ind</t>
   </si>
 </sst>
 </file>
@@ -2536,7 +2539,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E48F8AD-971A-4094-8D85-72B0AE25E8BF}">
   <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="114" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScale="114" workbookViewId="0">
       <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
@@ -3008,8 +3011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC51F965-835D-4E82-9AC8-2752CA30592B}">
   <dimension ref="A1:AJ257"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C103" zoomScale="98" zoomScaleNormal="25" workbookViewId="0">
-      <selection activeCell="G110" sqref="G110:R114"/>
+    <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="25" workbookViewId="0">
+      <selection activeCell="R115" sqref="C2:R115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9477,23 +9480,57 @@
       <c r="A115" s="12" t="s">
         <v>398</v>
       </c>
-      <c r="B115" s="14"/>
-      <c r="C115" s="8"/>
-      <c r="D115" s="8"/>
-      <c r="E115" s="8"/>
-      <c r="F115" s="8"/>
-      <c r="G115" s="8"/>
-      <c r="H115" s="8"/>
-      <c r="I115" s="8"/>
-      <c r="J115" s="8"/>
-      <c r="K115" s="8"/>
-      <c r="L115" s="8"/>
-      <c r="M115" s="8"/>
-      <c r="N115" s="8"/>
-      <c r="O115" s="8"/>
-      <c r="P115" s="8"/>
-      <c r="Q115" s="8"/>
-      <c r="R115" s="8"/>
+      <c r="B115" s="14" t="s">
+        <v>643</v>
+      </c>
+      <c r="C115" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="D115" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="E115" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="F115" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="G115" s="9" t="s">
+        <v>319</v>
+      </c>
+      <c r="H115" s="9" t="s">
+        <v>335</v>
+      </c>
+      <c r="I115" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="J115" s="9" t="s">
+        <v>552</v>
+      </c>
+      <c r="K115" s="9" t="s">
+        <v>335</v>
+      </c>
+      <c r="L115" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="M115" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="N115" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="O115" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="P115" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q115" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="R115" s="10" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="116" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A116" s="12" t="s">

</xml_diff>